<commit_message>
updated fake_data.csv and energy_inputs_to_model_with_fuel_conversion.xlsx for rail freight and rail passenger disesel and electric efficiencies
</commit_message>
<xml_diff>
--- a/ref/data_tables_and_derivations/ENERGY/energy_inputs_to_model_with_fuel_conversion_factors.xlsx
+++ b/ref/data_tables_and_derivations/ENERGY/energy_inputs_to_model_with_fuel_conversion_factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/FY21/SWCHE131_1000/Data/Energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/data_tables_and_derivations/ENERGY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642314C5-EBE2-644F-A5C2-9940C1539B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD46F6AE-B4E3-3A4F-9C4F-6B1EE7D3470E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="500" windowWidth="25880" windowHeight="13700" activeTab="6" xr2:uid="{5FFDFBED-0EDA-184B-B159-D6A0BE4DEBC4}"/>
+    <workbookView xWindow="1740" yWindow="500" windowWidth="26300" windowHeight="20260" firstSheet="6" activeTab="13" xr2:uid="{5FFDFBED-0EDA-184B-B159-D6A0BE4DEBC4}"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <sheet name="biomass_price" sheetId="9" r:id="rId11"/>
     <sheet name="natural_gas_price" sheetId="7" r:id="rId12"/>
     <sheet name="prices" sheetId="14" r:id="rId13"/>
+    <sheet name="rail_efficiencies" sheetId="15" r:id="rId14"/>
+    <sheet name="public_efficiencies" sheetId="16" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">prices!$A$1:$T$26</definedName>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="539">
   <si>
     <t>IEA World Energy Balance includes production by PJ. These sheets contain information to convert PJ to tonnes and m3 to tonnes</t>
   </si>
@@ -1583,12 +1585,241 @@
   <si>
     <t>$/MMBTU</t>
   </si>
+  <si>
+    <t>km/kwh dies</t>
+  </si>
+  <si>
+    <t>kwh/litre</t>
+  </si>
+  <si>
+    <t>mj/kwh</t>
+  </si>
+  <si>
+    <t>mj/litre</t>
+  </si>
+  <si>
+    <t>km/litre</t>
+  </si>
+  <si>
+    <t>km/kwh</t>
+  </si>
+  <si>
+    <t>elec</t>
+  </si>
+  <si>
+    <t>from https://www.eesi.org/articles/view/electrification-of-u.s.-railways-pie-in-the-sky-or-realistic-goal: 30-35 percent of energy in diesel reaches wheels; in elec, it reaches 95%)</t>
+  </si>
+  <si>
+    <t>0.0345 kWh revenue-tonne-km–1 with LFP technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.014 kWh tonne-km–1 </t>
+  </si>
+  <si>
+    <t>additional estimate for battery electric with regenerative braking</t>
+  </si>
+  <si>
+    <t>Our analysis is based on a representative Class I train operating in California, with four 3.3-MW locomotives pulling 100 boxcars and 6,806 revenue-tonnes (or tonnes of payload). A standard 14.6-m boxcar has a rated payload capacity of 114 t</t>
+  </si>
+  <si>
+    <t>kwh/revenue tonne km</t>
+  </si>
+  <si>
+    <t>kwh/km</t>
+  </si>
+  <si>
+    <t>revenue tonne</t>
+  </si>
+  <si>
+    <t>km/mj</t>
+  </si>
+  <si>
+    <t>ELECTRIC</t>
+  </si>
+  <si>
+    <t>NOTE:</t>
+  </si>
+  <si>
+    <t>"The energy consumed by battery freight trains increases by 5% (241-km range) because of the additional battery weight but it is still about half the energy consumed by diesel trains owing to the high efficiency of all-electric drives. "</t>
+  </si>
+  <si>
+    <t>factor_diesel</t>
+  </si>
+  <si>
+    <t>FREIGHT</t>
+  </si>
+  <si>
+    <t>https://japh.tums.ac.ir/index.php/japh/article/view/86</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SOURCE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: https://www.nature.com/articles/s41560-021-00915-5
+Popovich, N.D., Rajagopal, D., Tasar, E. et al. Economic, environmental and grid-resilience benefits of converting diesel trains to battery-electric. 
+Nat Energy 6, 1017–1025 (2021). https://doi.org/10.1038/s41560-021-00915-5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SOURCE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: https://japh.tums.ac.ir/index.php/japh/article/view/86
+Talaiekhozani A, Ghaffarpassand O, Talaei MR, Neshat N, Eydivandi B. EVALUATION OF EMISSION INVENTORY OF AIR POLLUTANTS FROM RAILROAD AND AIR TRANSPORTATION IN ISFAHAN METROPOLITAN IN 2016. JAPH. 2017;2(1).</t>
+    </r>
+  </si>
+  <si>
+    <t>litre/km</t>
+  </si>
+  <si>
+    <t>implied km/kwh</t>
+  </si>
+  <si>
+    <t>fuelefficiency_trns_rail_freight_diesel_km_per_litre</t>
+  </si>
+  <si>
+    <t>elecfuelefficiency_trns_rail_freight_km_per_kwh</t>
+  </si>
+  <si>
+    <t>max_2050</t>
+  </si>
+  <si>
+    <t>min_2050</t>
+  </si>
+  <si>
+    <t>METRO RAIL (subway, light rail)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SOURCE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: https://www.sciencedirect.com/science/article/abs/pii/S0959652620300081
+W.M. To, Peter K.C. Lee, Billy T.W. Yu, Sustainability assessment of an urban rail system – The case of Hong Kong, Journal of Cleaner Production, Volume 253, 2020, 119961, ISSN 0959-6526, https://doi.org/10.1016/j.jclepro.2020.119961.</t>
+    </r>
+  </si>
+  <si>
+    <t>Hong Kong Urban Rail Transit</t>
+  </si>
+  <si>
+    <t>kwh/pkm</t>
+  </si>
+  <si>
+    <t>0.076-0.093</t>
+  </si>
+  <si>
+    <t>LAM (cited in To et al. Kenworthy (2008) from https://www.sciencedirect.com/science/article/pii/B9780080453415000098)</t>
+  </si>
+  <si>
+    <t>mj/pkm</t>
+  </si>
+  <si>
+    <t>NOTE: "This figure shows that when load factor increases, energy efficiency improves because the rail system consumes less MJ per pkm."</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>hong kong</t>
+  </si>
+  <si>
+    <t>shanghai</t>
+  </si>
+  <si>
+    <t>USE REG IN PYTHON</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INV </t>
+  </si>
+  <si>
+    <t>LAC EST AVG LOAD</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>HONG KONG</t>
+  </si>
+  <si>
+    <t>avg person/train-car</t>
+  </si>
+  <si>
+    <t>PASSENGER</t>
+  </si>
+  <si>
+    <t>ELECTRICITY (EST)</t>
+  </si>
+  <si>
+    <t>fuelefficiency_trns_rail_passenger_diesel_km_per_litre</t>
+  </si>
+  <si>
+    <t>elecfuelefficiency_trns_rail_passenger_km_per_kwh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1686,6 +1917,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -1919,7 +2164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1991,32 +2236,14 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2024,13 +2251,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2039,14 +2263,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2077,6 +2322,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2244,6 +2522,55 @@
         <a:xfrm>
           <a:off x="10655300" y="266700"/>
           <a:ext cx="4579314" cy="6159500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1282700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>543811</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>108052</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38A49AB6-A994-FA5F-4375-FDCC5B4719A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3987800" y="3568700"/>
+          <a:ext cx="5636511" cy="4222852"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3874,6 +4201,756 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F50D75-3216-704D-87F9-6F7CF1AE4454}">
+  <dimension ref="A1:K75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="51.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C3">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>487</v>
+      </c>
+      <c r="C4" s="34">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>486</v>
+      </c>
+      <c r="D5">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>485</v>
+      </c>
+      <c r="C6">
+        <f>C4/D5</f>
+        <v>10.111111111111111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>484</v>
+      </c>
+      <c r="C7">
+        <f>C3/C6</f>
+        <v>0.87032967032967046</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="77" t="s">
+        <v>504</v>
+      </c>
+      <c r="B13" s="77"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="77"/>
+    </row>
+    <row r="17" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A17" s="78" t="s">
+        <v>504</v>
+      </c>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+    </row>
+    <row r="18" spans="1:11" s="80" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A18" s="79"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+    </row>
+    <row r="19" spans="1:11" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="82" t="s">
+        <v>506</v>
+      </c>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+    </row>
+    <row r="21" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="56" t="s">
+        <v>495</v>
+      </c>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="K21">
+        <f>47951850/5462141</f>
+        <v>8.7789476690550465</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>493</v>
+      </c>
+      <c r="C23" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>496</v>
+      </c>
+      <c r="C25" s="69" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>6806</v>
+      </c>
+      <c r="B26" t="s">
+        <v>498</v>
+      </c>
+      <c r="C26" s="69"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <f>A25*A26</f>
+        <v>234.80700000000002</v>
+      </c>
+      <c r="B27" t="s">
+        <v>497</v>
+      </c>
+      <c r="C27" s="69"/>
+      <c r="G27">
+        <f>1/8.8</f>
+        <v>0.11363636363636363</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="18">
+        <f>1/A27</f>
+        <v>4.2588168155123143E-3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>489</v>
+      </c>
+      <c r="C28" s="69"/>
+      <c r="D28">
+        <f>8.8/6806</f>
+        <v>1.2929767851895388E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="76">
+        <f>A28/D5</f>
+        <v>1.1830046709756428E-3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>499</v>
+      </c>
+      <c r="C29" s="69"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>0.5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>503</v>
+      </c>
+      <c r="C32" s="69" t="s">
+        <v>201</v>
+      </c>
+      <c r="D32" t="s">
+        <v>501</v>
+      </c>
+      <c r="E32" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f>A29*A32</f>
+        <v>5.9150233548782138E-4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>499</v>
+      </c>
+      <c r="C33" s="69"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="18">
+        <f>A33*C4</f>
+        <v>2.1530685011756697E-2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>488</v>
+      </c>
+      <c r="C34" s="69"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="82" t="s">
+        <v>507</v>
+      </c>
+      <c r="B39" s="81"/>
+      <c r="C39" s="81"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="81"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="81"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <f>ROUND(47951850/5462141,1)</f>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B41" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="18">
+        <f>1/A41</f>
+        <v>0.11363636363636363</v>
+      </c>
+      <c r="B42" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="18">
+        <f>A42*(A28/A34)</f>
+        <v>2.247752247752248E-2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="84"/>
+      <c r="B46" s="84" t="s">
+        <v>512</v>
+      </c>
+      <c r="C46" s="84" t="s">
+        <v>513</v>
+      </c>
+      <c r="D46" s="84" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="85" t="s">
+        <v>510</v>
+      </c>
+      <c r="B47" s="84">
+        <f>ROUND(A42/D47,2)</f>
+        <v>1.68</v>
+      </c>
+      <c r="C47" s="84">
+        <f>ROUND(A34/D47,2)</f>
+        <v>0.32</v>
+      </c>
+      <c r="D47" s="84">
+        <f>AVERAGE(A42,A34)</f>
+        <v>6.758352432406016E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="85" t="s">
+        <v>511</v>
+      </c>
+      <c r="B48" s="84">
+        <f>ROUND(A44/D48,2)</f>
+        <v>1.68</v>
+      </c>
+      <c r="C48" s="84">
+        <f>ROUND(A28/D48,2)</f>
+        <v>0.32</v>
+      </c>
+      <c r="D48" s="84">
+        <f>AVERAGE(A44,A28)</f>
+        <v>1.3368169646517398E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="26" x14ac:dyDescent="0.3">
+      <c r="A52" s="78" t="s">
+        <v>535</v>
+      </c>
+      <c r="B52" s="78"/>
+      <c r="C52" s="78"/>
+      <c r="D52" s="78"/>
+      <c r="E52" s="78"/>
+      <c r="F52" s="78"/>
+      <c r="G52" s="78"/>
+      <c r="H52" s="78"/>
+      <c r="I52" s="78"/>
+      <c r="J52" s="78"/>
+    </row>
+    <row r="53" spans="1:10" s="80" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A53" s="79"/>
+      <c r="B53" s="79"/>
+      <c r="C53" s="79"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="79"/>
+      <c r="F53" s="79"/>
+      <c r="G53" s="79"/>
+      <c r="H53" s="79"/>
+      <c r="I53" s="79"/>
+      <c r="J53" s="79"/>
+    </row>
+    <row r="54" spans="1:10" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="82" t="s">
+        <v>507</v>
+      </c>
+      <c r="B54" s="81"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
+      <c r="F54" s="81"/>
+      <c r="G54" s="81"/>
+      <c r="H54" s="81"/>
+      <c r="I54" s="81"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <f>ROUND(7235100/2282156,1)</f>
+        <v>3.2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>508</v>
+      </c>
+      <c r="C57" s="69" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <f>1/A57</f>
+        <v>0.3125</v>
+      </c>
+      <c r="B58" t="s">
+        <v>488</v>
+      </c>
+      <c r="C58" s="69"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <f>(A28/A34)*A58</f>
+        <v>6.1813186813186816E-2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="87"/>
+      <c r="B64" s="84" t="s">
+        <v>512</v>
+      </c>
+      <c r="C64" s="84" t="s">
+        <v>513</v>
+      </c>
+      <c r="D64" s="84" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="85" t="s">
+        <v>537</v>
+      </c>
+      <c r="B65" s="84">
+        <f>B47</f>
+        <v>1.68</v>
+      </c>
+      <c r="C65" s="84">
+        <f>C47</f>
+        <v>0.32</v>
+      </c>
+      <c r="D65" s="84">
+        <f>AVERAGE(A58)</f>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="85" t="s">
+        <v>538</v>
+      </c>
+      <c r="B66" s="84">
+        <f>B48</f>
+        <v>1.68</v>
+      </c>
+      <c r="C66" s="84">
+        <f>C48</f>
+        <v>0.32</v>
+      </c>
+      <c r="D66" s="84">
+        <f>AVERAGE(A60)</f>
+        <v>6.1813186813186816E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="87"/>
+      <c r="B71" s="84" t="s">
+        <v>512</v>
+      </c>
+      <c r="C71" s="84" t="s">
+        <v>513</v>
+      </c>
+      <c r="D71" s="84" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="85" t="s">
+        <v>510</v>
+      </c>
+      <c r="B72" s="84">
+        <v>1.68</v>
+      </c>
+      <c r="C72" s="84">
+        <v>0.32</v>
+      </c>
+      <c r="D72" s="84">
+        <v>6.758352432406016E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="85" t="s">
+        <v>511</v>
+      </c>
+      <c r="B73" s="84">
+        <v>1.68</v>
+      </c>
+      <c r="C73" s="84">
+        <v>0.32</v>
+      </c>
+      <c r="D73" s="84">
+        <v>1.3368169646517398E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="88" t="s">
+        <v>537</v>
+      </c>
+      <c r="B74" s="86">
+        <v>1.68</v>
+      </c>
+      <c r="C74" s="86">
+        <v>0.32</v>
+      </c>
+      <c r="D74" s="86">
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="88" t="s">
+        <v>538</v>
+      </c>
+      <c r="B75" s="86">
+        <v>1.68</v>
+      </c>
+      <c r="C75" s="86">
+        <v>0.32</v>
+      </c>
+      <c r="D75" s="86">
+        <v>6.1813186813186816E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A39:I39"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="A52:J52"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A19:I19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201F496F-0260-FD4C-850F-564E18865F2A}">
+  <dimension ref="A9:O32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="13" max="15" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="1:10" ht="26" x14ac:dyDescent="0.3">
+      <c r="A9" s="78" t="s">
+        <v>514</v>
+      </c>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
+    </row>
+    <row r="10" spans="1:10" s="80" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+    </row>
+    <row r="11" spans="1:10" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="82" t="s">
+        <v>515</v>
+      </c>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>518</v>
+      </c>
+      <c r="B14" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f>C32</f>
+        <v>71.146490917702906</v>
+      </c>
+      <c r="B18" t="s">
+        <v>534</v>
+      </c>
+      <c r="C18" t="s">
+        <v>522</v>
+      </c>
+      <c r="D18" t="s">
+        <v>523</v>
+      </c>
+      <c r="M18" s="65" t="s">
+        <v>521</v>
+      </c>
+      <c r="N18" s="65"/>
+      <c r="O18" s="65"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>25.8</v>
+      </c>
+      <c r="D19">
+        <v>0.5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>524</v>
+      </c>
+      <c r="M19" s="65"/>
+      <c r="N19" s="65"/>
+      <c r="O19" s="65"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>59.7</v>
+      </c>
+      <c r="D20">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E20" t="s">
+        <v>525</v>
+      </c>
+      <c r="M20" s="65"/>
+      <c r="N20" s="65"/>
+      <c r="O20" s="65"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>82</v>
+      </c>
+      <c r="D21">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="E21" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>528</v>
+      </c>
+      <c r="D24" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="C25" s="83">
+        <v>-7.0092399999999999E-3</v>
+      </c>
+      <c r="D25">
+        <v>0.68868282999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <f>1/C25</f>
+        <v>-142.66882001472342</v>
+      </c>
+      <c r="D28">
+        <f>D25/C25</f>
+        <v>-98.253566720500359</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <f>D19*C28-D28</f>
+        <v>26.919156713138648</v>
+      </c>
+      <c r="D30" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <f>D20*C28-D28</f>
+        <v>56.879608916230566</v>
+      </c>
+      <c r="D31" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>531</v>
+      </c>
+      <c r="C32">
+        <f>C28*A17-D28</f>
+        <v>71.146490917702906</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="M18:O20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881E6503-80B4-134F-BEAF-440BF1CB0F2D}">
   <dimension ref="A1:V81"/>
@@ -4001,19 +5078,19 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
       <c r="L11" t="s">
         <v>90</v>
       </c>
@@ -4037,42 +5114,42 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="174" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="50"/>
-      <c r="S15" s="50"/>
-      <c r="T15" s="50"/>
-      <c r="U15" s="50"/>
-      <c r="V15" s="50"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="56"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="56"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="56"/>
+      <c r="V15" s="56"/>
     </row>
     <row r="16" spans="1:22" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="55"/>
-      <c r="R16" s="55"/>
-      <c r="S16" s="55"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="57"/>
+      <c r="S16" s="57"/>
       <c r="T16" s="18"/>
       <c r="U16" s="18"/>
     </row>
@@ -4119,7 +5196,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="53" t="s">
         <v>88</v>
       </c>
       <c r="B18" t="s">
@@ -4173,7 +5250,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="52"/>
+      <c r="A19" s="53"/>
       <c r="B19" t="s">
         <v>36</v>
       </c>
@@ -4225,7 +5302,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="52"/>
+      <c r="A20" s="53"/>
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -4277,7 +5354,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21" s="52"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="8" t="s">
         <v>85</v>
       </c>
@@ -4326,7 +5403,7 @@
       <c r="S21" s="8"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A22" s="52"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="8" t="s">
         <v>86</v>
       </c>
@@ -4357,7 +5434,7 @@
       <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A23" s="52"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="8" t="s">
         <v>87</v>
       </c>
@@ -4389,7 +5466,7 @@
       <c r="S23" s="8"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="52"/>
+      <c r="A24" s="53"/>
       <c r="B24" t="s">
         <v>39</v>
       </c>
@@ -4413,7 +5490,7 @@
       <c r="A25" s="20"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="53" t="s">
         <v>89</v>
       </c>
       <c r="B26" t="s">
@@ -4436,7 +5513,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A27" s="52"/>
+      <c r="A27" s="53"/>
       <c r="B27" t="s">
         <v>91</v>
       </c>
@@ -4463,10 +5540,10 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C28" s="8"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="51"/>
+      <c r="N28" s="61"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="61"/>
+      <c r="Q28" s="61"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C29" s="8"/>
@@ -4484,13 +5561,13 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J30" s="54" t="s">
+      <c r="J30" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="K30" s="56" t="s">
+      <c r="K30" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="L30" s="57"/>
+      <c r="L30" s="51"/>
       <c r="M30" s="58"/>
       <c r="N30" s="9">
         <v>7.0000000000000007E-2</v>
@@ -4506,12 +5583,12 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J31" s="54"/>
-      <c r="K31" s="59" t="s">
+      <c r="J31" s="63"/>
+      <c r="K31" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="L31" s="52"/>
-      <c r="M31" s="60"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="59"/>
       <c r="N31" s="12">
         <v>0.83</v>
       </c>
@@ -4530,12 +5607,12 @@
         <f>(0.0022*0.037)^0.5</f>
         <v>9.0221948549119683E-3</v>
       </c>
-      <c r="J32" s="54"/>
-      <c r="K32" s="61" t="s">
+      <c r="J32" s="63"/>
+      <c r="K32" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="L32" s="62"/>
-      <c r="M32" s="63"/>
+      <c r="L32" s="55"/>
+      <c r="M32" s="60"/>
       <c r="N32" s="14">
         <v>0.1</v>
       </c>
@@ -4550,13 +5627,13 @@
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J33" s="53" t="s">
+      <c r="J33" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="K33" s="56" t="s">
+      <c r="K33" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="L33" s="57"/>
+      <c r="L33" s="51"/>
       <c r="M33" s="58"/>
       <c r="N33" s="9">
         <v>0.09</v>
@@ -4572,12 +5649,12 @@
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J34" s="53"/>
-      <c r="K34" s="59" t="s">
+      <c r="J34" s="49"/>
+      <c r="K34" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="L34" s="52"/>
-      <c r="M34" s="60"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="59"/>
       <c r="N34" s="12">
         <v>0.78</v>
       </c>
@@ -4592,12 +5669,12 @@
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J35" s="53"/>
-      <c r="K35" s="61" t="s">
+      <c r="J35" s="49"/>
+      <c r="K35" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="L35" s="62"/>
-      <c r="M35" s="63"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="60"/>
       <c r="N35" s="14">
         <v>0.13</v>
       </c>
@@ -4612,13 +5689,13 @@
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J36" s="53" t="s">
+      <c r="J36" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="K36" s="56" t="s">
+      <c r="K36" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="L36" s="57"/>
+      <c r="L36" s="51"/>
       <c r="M36" s="58"/>
       <c r="N36" s="9">
         <v>0.2</v>
@@ -4634,12 +5711,12 @@
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J37" s="53"/>
-      <c r="K37" s="59" t="s">
+      <c r="J37" s="49"/>
+      <c r="K37" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="L37" s="52"/>
-      <c r="M37" s="60"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="59"/>
       <c r="N37" s="12">
         <v>0.8</v>
       </c>
@@ -4654,12 +5731,12 @@
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J38" s="53"/>
-      <c r="K38" s="61" t="s">
+      <c r="J38" s="49"/>
+      <c r="K38" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="L38" s="62"/>
-      <c r="M38" s="63"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="60"/>
       <c r="N38" s="12">
         <v>0</v>
       </c>
@@ -4674,14 +5751,14 @@
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J39" s="53" t="s">
+      <c r="J39" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="K39" s="56" t="s">
+      <c r="K39" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="L39" s="57"/>
-      <c r="M39" s="57"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
       <c r="N39" s="9">
         <f>AVERAGE(N30,N33,N36)</f>
         <v>0.12</v>
@@ -4700,12 +5777,12 @@
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J40" s="53"/>
-      <c r="K40" s="59" t="s">
+      <c r="J40" s="49"/>
+      <c r="K40" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
       <c r="N40" s="12">
         <f t="shared" ref="N40:Q41" si="5">AVERAGE(N31,N34,N37)</f>
         <v>0.80333333333333334</v>
@@ -4724,12 +5801,12 @@
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J41" s="53"/>
-      <c r="K41" s="61" t="s">
+      <c r="J41" s="49"/>
+      <c r="K41" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="L41" s="62"/>
-      <c r="M41" s="62"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="55"/>
       <c r="N41" s="14">
         <f t="shared" si="5"/>
         <v>7.6666666666666675E-2</v>
@@ -4776,14 +5853,14 @@
       <c r="G43" t="s">
         <v>47</v>
       </c>
-      <c r="I43" s="65" t="s">
+      <c r="I43" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="J43" s="65"/>
-      <c r="K43" s="65"/>
-      <c r="L43" s="65"/>
-      <c r="M43" s="65"/>
-      <c r="N43" s="64">
+      <c r="J43" s="48"/>
+      <c r="K43" s="48"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="47">
         <f>1-N42</f>
         <v>8.7121212121212155E-2</v>
       </c>
@@ -4808,12 +5885,12 @@
         <f>F43-F22-F23</f>
         <v>6.8000000000000027E-8</v>
       </c>
-      <c r="I44" s="65"/>
-      <c r="J44" s="65"/>
-      <c r="K44" s="65"/>
-      <c r="L44" s="65"/>
-      <c r="M44" s="65"/>
-      <c r="N44" s="64"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
+      <c r="K44" s="48"/>
+      <c r="L44" s="48"/>
+      <c r="M44" s="48"/>
+      <c r="N44" s="47"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
@@ -4930,19 +6007,19 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="47" t="s">
+      <c r="A51" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="B51" s="47"/>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="47"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="62"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="62"/>
+      <c r="H51" s="62"/>
+      <c r="I51" s="62"/>
+      <c r="J51" s="62"/>
+      <c r="K51" s="62"/>
     </row>
     <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="26" t="s">
@@ -4961,19 +6038,19 @@
     </row>
     <row r="56" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="47" t="s">
+      <c r="A57" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="47"/>
-      <c r="F57" s="47"/>
-      <c r="G57" s="47"/>
-      <c r="H57" s="47"/>
-      <c r="I57" s="47"/>
-      <c r="J57" s="47"/>
-      <c r="K57" s="47"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="62"/>
+      <c r="G57" s="62"/>
+      <c r="H57" s="62"/>
+      <c r="I57" s="62"/>
+      <c r="J57" s="62"/>
+      <c r="K57" s="62"/>
     </row>
     <row r="58" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="26" t="s">
@@ -4999,34 +6076,34 @@
       </c>
     </row>
     <row r="64" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A64" s="47" t="s">
+      <c r="A64" s="62" t="s">
         <v>280</v>
       </c>
-      <c r="B64" s="47"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="47"/>
-      <c r="H64" s="47"/>
-      <c r="I64" s="47"/>
-      <c r="J64" s="47"/>
-      <c r="K64" s="47"/>
+      <c r="B64" s="62"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="62"/>
+      <c r="E64" s="62"/>
+      <c r="F64" s="62"/>
+      <c r="G64" s="62"/>
+      <c r="H64" s="62"/>
+      <c r="I64" s="62"/>
+      <c r="J64" s="62"/>
+      <c r="K64" s="62"/>
     </row>
     <row r="71" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A71" s="47" t="s">
+      <c r="A71" s="62" t="s">
         <v>315</v>
       </c>
-      <c r="B71" s="47"/>
-      <c r="C71" s="47"/>
-      <c r="D71" s="47"/>
-      <c r="E71" s="47"/>
-      <c r="F71" s="47"/>
-      <c r="G71" s="47"/>
-      <c r="H71" s="47"/>
-      <c r="I71" s="47"/>
-      <c r="J71" s="47"/>
-      <c r="K71" s="47"/>
+      <c r="B71" s="62"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="62"/>
+      <c r="E71" s="62"/>
+      <c r="F71" s="62"/>
+      <c r="G71" s="62"/>
+      <c r="H71" s="62"/>
+      <c r="I71" s="62"/>
+      <c r="J71" s="62"/>
+      <c r="K71" s="62"/>
     </row>
     <row r="72" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="26" t="s">
@@ -5039,10 +6116,10 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="48" t="s">
+      <c r="A74" s="64" t="s">
         <v>309</v>
       </c>
-      <c r="B74" s="48"/>
+      <c r="B74" s="64"/>
       <c r="C74" s="42" t="s">
         <v>109</v>
       </c>
@@ -5067,10 +6144,10 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" s="48" t="s">
+      <c r="A76" s="64" t="s">
         <v>317</v>
       </c>
-      <c r="B76" s="48"/>
+      <c r="B76" s="64"/>
       <c r="C76" s="41">
         <f>C75*$B$80</f>
         <v>2.6086956521739112E-4</v>
@@ -5141,12 +6218,21 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="N43:N44"/>
-    <mergeCell ref="I43:M44"/>
-    <mergeCell ref="J39:J41"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="A71:K71"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="A64:K64"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="J36:J38"/>
+    <mergeCell ref="J33:J35"/>
+    <mergeCell ref="J30:J32"/>
     <mergeCell ref="N15:V15"/>
     <mergeCell ref="R16:S16"/>
     <mergeCell ref="K36:M36"/>
@@ -5160,21 +6246,12 @@
     <mergeCell ref="N28:Q28"/>
     <mergeCell ref="K34:M34"/>
     <mergeCell ref="K35:M35"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="J36:J38"/>
-    <mergeCell ref="J33:J35"/>
-    <mergeCell ref="J30:J32"/>
-    <mergeCell ref="A71:K71"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="A64:K64"/>
-    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="N43:N44"/>
+    <mergeCell ref="I43:M44"/>
+    <mergeCell ref="J39:J41"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="K41:M41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A55" r:id="rId1" xr:uid="{939BE22A-9CE0-E745-AEFB-468D46C49282}"/>
@@ -5439,31 +6516,31 @@
       <c r="N5" s="44"/>
     </row>
     <row r="6" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
       <c r="L6" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
@@ -5493,7 +6570,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="53" t="s">
         <v>88</v>
       </c>
       <c r="B9" t="s">
@@ -5535,7 +6612,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
+      <c r="A10" s="53"/>
       <c r="B10" t="s">
         <v>122</v>
       </c>
@@ -5579,7 +6656,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="52"/>
+      <c r="A11" s="53"/>
       <c r="B11" t="s">
         <v>123</v>
       </c>
@@ -5619,7 +6696,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="52"/>
+      <c r="A12" s="53"/>
       <c r="B12" t="s">
         <v>124</v>
       </c>
@@ -5663,7 +6740,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
+      <c r="A13" s="53"/>
       <c r="B13" t="s">
         <v>125</v>
       </c>
@@ -5685,7 +6762,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="53" t="s">
         <v>89</v>
       </c>
       <c r="B14" t="s">
@@ -5723,7 +6800,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="52"/>
+      <c r="A15" s="53"/>
       <c r="B15" t="s">
         <v>129</v>
       </c>
@@ -5759,7 +6836,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
+      <c r="A16" s="53"/>
       <c r="B16" t="s">
         <v>126</v>
       </c>
@@ -5795,7 +6872,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="52"/>
+      <c r="A17" s="53"/>
       <c r="B17" t="s">
         <v>127</v>
       </c>
@@ -5832,19 +6909,19 @@
     </row>
     <row r="18" spans="1:15" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="62" t="s">
         <v>303</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
     </row>
     <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
@@ -5945,7 +7022,7 @@
         <v>1.2723422278695466</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="119" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="85" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>145</v>
       </c>
@@ -5972,10 +7049,10 @@
       <c r="B34">
         <v>408.31599999999997</v>
       </c>
-      <c r="D34" s="48" t="s">
+      <c r="D34" s="64" t="s">
         <v>309</v>
       </c>
-      <c r="E34" s="48"/>
+      <c r="E34" s="64"/>
       <c r="F34" s="42" t="s">
         <v>109</v>
       </c>
@@ -6016,10 +7093,10 @@
         <f>B34/B35</f>
         <v>1.6789999588798881E-2</v>
       </c>
-      <c r="D36" s="48" t="s">
+      <c r="D36" s="64" t="s">
         <v>313</v>
       </c>
-      <c r="E36" s="48"/>
+      <c r="E36" s="64"/>
       <c r="F36" s="41">
         <f>F35*B36</f>
         <v>3.3579999177597762E-5</v>
@@ -6064,19 +7141,19 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="62"/>
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="26" t="s">
@@ -6320,34 +7397,34 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="62"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="G16" s="51" t="s">
+      <c r="G16" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="N16" s="51" t="s">
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="N16" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="61"/>
       <c r="S16" s="23"/>
       <c r="T16" s="23"/>
       <c r="U16" s="23"/>
@@ -6952,19 +8029,19 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="47" t="s">
+      <c r="A34" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="62"/>
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="26"/>
@@ -6974,19 +8051,19 @@
     </row>
     <row r="39" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="62"/>
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="26"/>
@@ -7164,7 +8241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376CCDCF-BF68-B44A-A3EA-06F3A7228FFF}">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+    <sheetView zoomScale="109" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -7179,21 +8256,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
@@ -7454,19 +8531,19 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A41" s="47" t="s">
+      <c r="A41" s="62" t="s">
         <v>314</v>
       </c>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="62"/>
+      <c r="J41" s="62"/>
+      <c r="K41" s="62"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -7501,7 +8578,7 @@
         <f>1/8.07</f>
         <v>0.12391573729863692</v>
       </c>
-      <c r="G47" s="51" t="s">
+      <c r="G47" s="61" t="s">
         <v>289</v>
       </c>
     </row>
@@ -7520,7 +8597,7 @@
         <f>1.06*E47</f>
         <v>0.13135068153655513</v>
       </c>
-      <c r="G48" s="51"/>
+      <c r="G48" s="61"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -7537,7 +8614,7 @@
         <f>E48*1.1</f>
         <v>0.14448574969021066</v>
       </c>
-      <c r="G49" s="51"/>
+      <c r="G49" s="61"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -7553,7 +8630,7 @@
       <c r="E50">
         <v>6</v>
       </c>
-      <c r="G50" s="51"/>
+      <c r="G50" s="61"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -9299,7 +10376,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>190</v>
       </c>
       <c r="B1" t="s">
@@ -9329,7 +10406,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
+      <c r="A2" s="53"/>
       <c r="B2" t="s">
         <v>189</v>
       </c>
@@ -9350,7 +10427,7 @@
       <c r="S2" s="36"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="52"/>
+      <c r="A3" s="53"/>
       <c r="B3" t="s">
         <v>162</v>
       </c>
@@ -9805,14 +10882,14 @@
       <c r="S29" s="36"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G30" s="51" t="s">
+      <c r="G30" s="61" t="s">
         <v>192</v>
       </c>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="51"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="61"/>
+      <c r="L30" s="61"/>
       <c r="N30" s="36"/>
       <c r="O30" s="36"/>
       <c r="P30" s="36"/>
@@ -9845,14 +10922,14 @@
       <c r="S33" s="36"/>
     </row>
     <row r="34" spans="14:19" x14ac:dyDescent="0.2">
-      <c r="N34" s="51" t="s">
+      <c r="N34" s="61" t="s">
         <v>191</v>
       </c>
-      <c r="O34" s="51"/>
-      <c r="P34" s="51"/>
-      <c r="Q34" s="51"/>
-      <c r="R34" s="51"/>
-      <c r="S34" s="51"/>
+      <c r="O34" s="61"/>
+      <c r="P34" s="61"/>
+      <c r="Q34" s="61"/>
+      <c r="R34" s="61"/>
+      <c r="S34" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
updated ENTC attribute to include subsector-level emission attributions from electricity generation
</commit_message>
<xml_diff>
--- a/ref/data_tables_and_derivations/ENERGY/energy_inputs_to_model_with_fuel_conversion_factors.xlsx
+++ b/ref/data_tables_and_derivations/ENERGY/energy_inputs_to_model_with_fuel_conversion_factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/data_tables_and_derivations/ENERGY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD46F6AE-B4E3-3A4F-9C4F-6B1EE7D3470E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB74293-E80E-2444-AE69-273B0FC8C615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="500" windowWidth="26300" windowHeight="20260" firstSheet="6" activeTab="13" xr2:uid="{5FFDFBED-0EDA-184B-B159-D6A0BE4DEBC4}"/>
+    <workbookView xWindow="4820" yWindow="500" windowWidth="26300" windowHeight="20260" firstSheet="6" activeTab="13" xr2:uid="{5FFDFBED-0EDA-184B-B159-D6A0BE4DEBC4}"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -4206,7 +4206,7 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+      <selection activeCell="C57" sqref="C57:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added emissions allocation in ENTC based on subsector energy demands and modified transformations to shift mode share based on percentage of modal demand, not pkm (added transfer_value_scalar option to transformation_general)
</commit_message>
<xml_diff>
--- a/ref/data_tables_and_derivations/ENERGY/energy_inputs_to_model_with_fuel_conversion_factors.xlsx
+++ b/ref/data_tables_and_derivations/ENERGY/energy_inputs_to_model_with_fuel_conversion_factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/data_tables_and_derivations/ENERGY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB74293-E80E-2444-AE69-273B0FC8C615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E9D0DB-141B-214D-96FE-3B42E3CE0AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="500" windowWidth="26300" windowHeight="20260" firstSheet="6" activeTab="13" xr2:uid="{5FFDFBED-0EDA-184B-B159-D6A0BE4DEBC4}"/>
+    <workbookView xWindow="4820" yWindow="500" windowWidth="26300" windowHeight="20260" firstSheet="6" activeTab="14" xr2:uid="{5FFDFBED-0EDA-184B-B159-D6A0BE4DEBC4}"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,8 @@
     <sheet name="natural_gas_price" sheetId="7" r:id="rId12"/>
     <sheet name="prices" sheetId="14" r:id="rId13"/>
     <sheet name="rail_efficiencies" sheetId="15" r:id="rId14"/>
-    <sheet name="public_efficiencies" sheetId="16" r:id="rId15"/>
+    <sheet name="aviation_freight" sheetId="17" r:id="rId15"/>
+    <sheet name="public_efficiencies" sheetId="16" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">prices!$A$1:$T$26</definedName>
@@ -51,8 +52,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="631">
   <si>
     <t>IEA World Energy Balance includes production by PJ. These sheets contain information to convert PJ to tonnes and m3 to tonnes</t>
   </si>
@@ -1814,12 +1837,300 @@
   <si>
     <t>elecfuelefficiency_trns_rail_passenger_km_per_kwh</t>
   </si>
+  <si>
+    <t>LOOSE NUMBERS FROM WIKIPEDIA</t>
+  </si>
+  <si>
+    <t>Aircraft</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>(m3)</t>
+  </si>
+  <si>
+    <t>Cruise</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Airbus A300-600F</t>
+  </si>
+  <si>
+    <t>48,000 kg (106,000 lb)</t>
+  </si>
+  <si>
+    <t>–</t>
+  </si>
+  <si>
+    <t>7,400 km (4,000 nmi)</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>Airbus A330-200F</t>
+  </si>
+  <si>
+    <t>70,000 kg (154,000 lb)</t>
+  </si>
+  <si>
+    <t>871 km/h (470 kn)</t>
+  </si>
+  <si>
+    <r>
+      <t>Airbus A380</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF795CB2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[24]</t>
+    </r>
+  </si>
+  <si>
+    <t>68,000 kg (150,000 lb)</t>
+  </si>
+  <si>
+    <t>13,300 km (8,000 nmi)</t>
+  </si>
+  <si>
+    <t>Airbus A400M</t>
+  </si>
+  <si>
+    <t>37,000 kg (82,000 lb)</t>
+  </si>
+  <si>
+    <t>780 km/h (420 kn)</t>
+  </si>
+  <si>
+    <t>6,390 km (3,450 nmi)</t>
+  </si>
+  <si>
+    <t>Military</t>
+  </si>
+  <si>
+    <t>Airbus Beluga</t>
+  </si>
+  <si>
+    <t>47,000 kg (104,000 lb)</t>
+  </si>
+  <si>
+    <t>4,632 km (2,500 nmi)</t>
+  </si>
+  <si>
+    <t>Airbus BelugaXL</t>
+  </si>
+  <si>
+    <t>53,000 kg (117,000 lb)</t>
+  </si>
+  <si>
+    <t>4,074 km (2,200 nmi)</t>
+  </si>
+  <si>
+    <t>Antonov An-22</t>
+  </si>
+  <si>
+    <t>80,000 kg (176,000 lb)</t>
+  </si>
+  <si>
+    <t>740 km/h (400 kn)</t>
+  </si>
+  <si>
+    <t>10,950 km (5,910 nmi)</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Antonov An-124</t>
+  </si>
+  <si>
+    <t>150,000 kg (331,000 lb)</t>
+  </si>
+  <si>
+    <t>800 km/h (430 kn)</t>
+  </si>
+  <si>
+    <t>5,400 km (2,900 nmi)</t>
+  </si>
+  <si>
+    <t>Antonov An-225</t>
+  </si>
+  <si>
+    <t>250,000 kg (551,000 lb)</t>
+  </si>
+  <si>
+    <t>15,400 km (8,316 nmi)</t>
+  </si>
+  <si>
+    <t>Boeing 737-700C</t>
+  </si>
+  <si>
+    <t>18,200 kg (40,000 lb)</t>
+  </si>
+  <si>
+    <t>931 km/h (503 kn)</t>
+  </si>
+  <si>
+    <t>5,330 km (2,880 nmi)</t>
+  </si>
+  <si>
+    <t>Boeing 747 LCF</t>
+  </si>
+  <si>
+    <t>83,325 kg (183,700 lb)</t>
+  </si>
+  <si>
+    <t>878 km/h (474 kn)</t>
+  </si>
+  <si>
+    <t>7,800 km (4,200 nmi)</t>
+  </si>
+  <si>
+    <t>Boeing 747-8F</t>
+  </si>
+  <si>
+    <t>134,200 kg (295,900 lb)</t>
+  </si>
+  <si>
+    <t>908 km/h (490 kn)</t>
+  </si>
+  <si>
+    <t>8,288 km (4,475 nmi)</t>
+  </si>
+  <si>
+    <t>Boeing 757-200F</t>
+  </si>
+  <si>
+    <t>39,780 kg (87,700 lb)</t>
+  </si>
+  <si>
+    <t>955 km/h (516 kn)</t>
+  </si>
+  <si>
+    <t>5,834 km (3,150 nmi)</t>
+  </si>
+  <si>
+    <t>Boeing 767-300F</t>
+  </si>
+  <si>
+    <t>52,700 kg (116,200 lb)</t>
+  </si>
+  <si>
+    <t>850 km/h (461 kn)</t>
+  </si>
+  <si>
+    <t>6,025 km (3,225 nmi)</t>
+  </si>
+  <si>
+    <t>Boeing 777F</t>
+  </si>
+  <si>
+    <t>103,000 kg (227,000 lb)</t>
+  </si>
+  <si>
+    <t>896 km/h (484 kn)</t>
+  </si>
+  <si>
+    <t>9,070 km (4,900 nmi)</t>
+  </si>
+  <si>
+    <t>Boeing C-17</t>
+  </si>
+  <si>
+    <t>77,519 kg (170,900 lb)</t>
+  </si>
+  <si>
+    <t>830 km/h (450 kn)</t>
+  </si>
+  <si>
+    <t>4,482 km (2,420 nmi)</t>
+  </si>
+  <si>
+    <t>Bombardier Dash 8-100</t>
+  </si>
+  <si>
+    <t>4,700 kg (10,400 lb)</t>
+  </si>
+  <si>
+    <t>491 km/h (265 kn)</t>
+  </si>
+  <si>
+    <t>2,039 km (1,100 nmi)</t>
+  </si>
+  <si>
+    <t>Douglas DC-10-30</t>
+  </si>
+  <si>
+    <t>77,000 kg (170,000 lb)</t>
+  </si>
+  <si>
+    <t>5,790 km (3,127 nmi)</t>
+  </si>
+  <si>
+    <t>Lockheed C-5</t>
+  </si>
+  <si>
+    <t>122,470 kg (270,000 lb)</t>
+  </si>
+  <si>
+    <t>919 km/h</t>
+  </si>
+  <si>
+    <t>4,440 km (2,400 nmi)</t>
+  </si>
+  <si>
+    <t>Lockheed C-130</t>
+  </si>
+  <si>
+    <t>20,400 kg (45,000 lb)</t>
+  </si>
+  <si>
+    <t>540 km/h (292 kn)</t>
+  </si>
+  <si>
+    <t>3,800 km (2,050 nmi)</t>
+  </si>
+  <si>
+    <t>McDonnell Douglas MD-11</t>
+  </si>
+  <si>
+    <t>91,670 kg (202,100 lb)</t>
+  </si>
+  <si>
+    <t>945 km/h (520 kn)</t>
+  </si>
+  <si>
+    <t>7,320 km (3,950 nmi)</t>
+  </si>
+  <si>
+    <t>Payload (kg)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Cargo_aircraft</t>
+  </si>
+  <si>
+    <t>PAYLOAD</t>
+  </si>
+  <si>
+    <t>MEDIAN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1930,6 +2241,32 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF795CB2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF795CB2"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2164,7 +2501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2236,14 +2573,51 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2251,10 +2625,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2263,35 +2640,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2323,39 +2679,23 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4205,7 +4545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F50D75-3216-704D-87F9-6F7CF1AE4454}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+    <sheetView topLeftCell="A54" workbookViewId="0">
       <selection activeCell="C57" sqref="C57:C58"/>
     </sheetView>
   </sheetViews>
@@ -4275,65 +4615,65 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="86" t="s">
         <v>504</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="77"/>
-      <c r="J13" s="77"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
     </row>
     <row r="17" spans="1:11" ht="26" x14ac:dyDescent="0.3">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="85" t="s">
         <v>504</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="78"/>
-    </row>
-    <row r="18" spans="1:11" s="80" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A18" s="79"/>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="79"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="85"/>
+    </row>
+    <row r="18" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:11" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="83" t="s">
         <v>506</v>
       </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="84"/>
     </row>
     <row r="21" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="57" t="s">
         <v>495</v>
       </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
       <c r="K21">
         <f>47951850/5462141</f>
         <v>8.7789476690550465</v>
@@ -4359,7 +4699,7 @@
       <c r="B25" t="s">
         <v>496</v>
       </c>
-      <c r="C25" s="69" t="s">
+      <c r="C25" s="76" t="s">
         <v>500</v>
       </c>
     </row>
@@ -4370,7 +4710,7 @@
       <c r="B26" t="s">
         <v>498</v>
       </c>
-      <c r="C26" s="69"/>
+      <c r="C26" s="76"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -4380,7 +4720,7 @@
       <c r="B27" t="s">
         <v>497</v>
       </c>
-      <c r="C27" s="69"/>
+      <c r="C27" s="76"/>
       <c r="G27">
         <f>1/8.8</f>
         <v>0.11363636363636363</v>
@@ -4394,21 +4734,21 @@
       <c r="B28" t="s">
         <v>489</v>
       </c>
-      <c r="C28" s="69"/>
+      <c r="C28" s="76"/>
       <c r="D28">
         <f>8.8/6806</f>
         <v>1.2929767851895388E-3</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="76">
+      <c r="A29">
         <f>A28/D5</f>
         <v>1.1830046709756428E-3</v>
       </c>
       <c r="B29" t="s">
         <v>499</v>
       </c>
-      <c r="C29" s="69"/>
+      <c r="C29" s="76"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -4417,7 +4757,7 @@
       <c r="B32" t="s">
         <v>503</v>
       </c>
-      <c r="C32" s="69" t="s">
+      <c r="C32" s="76" t="s">
         <v>201</v>
       </c>
       <c r="D32" t="s">
@@ -4435,7 +4775,7 @@
       <c r="B33" t="s">
         <v>499</v>
       </c>
-      <c r="C33" s="69"/>
+      <c r="C33" s="76"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
@@ -4445,7 +4785,7 @@
       <c r="B34" t="s">
         <v>488</v>
       </c>
-      <c r="C34" s="69"/>
+      <c r="C34" s="76"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
@@ -4453,17 +4793,17 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="82" t="s">
+      <c r="A39" s="83" t="s">
         <v>507</v>
       </c>
-      <c r="B39" s="81"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="81"/>
+      <c r="B39" s="84"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="84"/>
+      <c r="H39" s="84"/>
+      <c r="I39" s="84"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -4493,89 +4833,89 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="84"/>
-      <c r="B46" s="84" t="s">
+      <c r="A46" s="49"/>
+      <c r="B46" s="49" t="s">
         <v>512</v>
       </c>
-      <c r="C46" s="84" t="s">
+      <c r="C46" s="49" t="s">
         <v>513</v>
       </c>
-      <c r="D46" s="84" t="s">
+      <c r="D46" s="49" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="85" t="s">
+      <c r="A47" s="50" t="s">
         <v>510</v>
       </c>
-      <c r="B47" s="84">
+      <c r="B47" s="49">
         <f>ROUND(A42/D47,2)</f>
         <v>1.68</v>
       </c>
-      <c r="C47" s="84">
+      <c r="C47" s="49">
         <f>ROUND(A34/D47,2)</f>
         <v>0.32</v>
       </c>
-      <c r="D47" s="84">
+      <c r="D47" s="49">
         <f>AVERAGE(A42,A34)</f>
         <v>6.758352432406016E-2</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="85" t="s">
+      <c r="A48" s="50" t="s">
         <v>511</v>
       </c>
-      <c r="B48" s="84">
+      <c r="B48" s="49">
         <f>ROUND(A44/D48,2)</f>
         <v>1.68</v>
       </c>
-      <c r="C48" s="84">
+      <c r="C48" s="49">
         <f>ROUND(A28/D48,2)</f>
         <v>0.32</v>
       </c>
-      <c r="D48" s="84">
+      <c r="D48" s="49">
         <f>AVERAGE(A44,A28)</f>
         <v>1.3368169646517398E-2</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="26" x14ac:dyDescent="0.3">
-      <c r="A52" s="78" t="s">
+      <c r="A52" s="85" t="s">
         <v>535</v>
       </c>
-      <c r="B52" s="78"/>
-      <c r="C52" s="78"/>
-      <c r="D52" s="78"/>
-      <c r="E52" s="78"/>
-      <c r="F52" s="78"/>
-      <c r="G52" s="78"/>
-      <c r="H52" s="78"/>
-      <c r="I52" s="78"/>
-      <c r="J52" s="78"/>
-    </row>
-    <row r="53" spans="1:10" s="80" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A53" s="79"/>
-      <c r="B53" s="79"/>
-      <c r="C53" s="79"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="79"/>
-      <c r="F53" s="79"/>
-      <c r="G53" s="79"/>
-      <c r="H53" s="79"/>
-      <c r="I53" s="79"/>
-      <c r="J53" s="79"/>
+      <c r="B52" s="85"/>
+      <c r="C52" s="85"/>
+      <c r="D52" s="85"/>
+      <c r="E52" s="85"/>
+      <c r="F52" s="85"/>
+      <c r="G52" s="85"/>
+      <c r="H52" s="85"/>
+      <c r="I52" s="85"/>
+      <c r="J52" s="85"/>
+    </row>
+    <row r="53" spans="1:10" ht="26" x14ac:dyDescent="0.3">
+      <c r="A53" s="47"/>
+      <c r="B53" s="47"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="47"/>
+      <c r="I53" s="47"/>
+      <c r="J53" s="47"/>
     </row>
     <row r="54" spans="1:10" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="82" t="s">
+      <c r="A54" s="83" t="s">
         <v>507</v>
       </c>
-      <c r="B54" s="81"/>
-      <c r="C54" s="81"/>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
-      <c r="F54" s="81"/>
-      <c r="G54" s="81"/>
-      <c r="H54" s="81"/>
-      <c r="I54" s="81"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="84"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="84"/>
+      <c r="F54" s="84"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="84"/>
+      <c r="I54" s="84"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
@@ -4585,7 +4925,7 @@
       <c r="B57" t="s">
         <v>508</v>
       </c>
-      <c r="C57" s="69" t="s">
+      <c r="C57" s="76" t="s">
         <v>201</v>
       </c>
     </row>
@@ -4597,7 +4937,7 @@
       <c r="B58" t="s">
         <v>488</v>
       </c>
-      <c r="C58" s="69"/>
+      <c r="C58" s="76"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
@@ -4609,137 +4949,865 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A64" s="87"/>
-      <c r="B64" s="84" t="s">
+      <c r="A64" s="52"/>
+      <c r="B64" s="49" t="s">
         <v>512</v>
       </c>
-      <c r="C64" s="84" t="s">
+      <c r="C64" s="49" t="s">
         <v>513</v>
       </c>
-      <c r="D64" s="84" t="s">
+      <c r="D64" s="49" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="85" t="s">
+      <c r="A65" s="50" t="s">
         <v>537</v>
       </c>
-      <c r="B65" s="84">
+      <c r="B65" s="49">
         <f>B47</f>
         <v>1.68</v>
       </c>
-      <c r="C65" s="84">
+      <c r="C65" s="49">
         <f>C47</f>
         <v>0.32</v>
       </c>
-      <c r="D65" s="84">
+      <c r="D65" s="49">
         <f>AVERAGE(A58)</f>
         <v>0.3125</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="85" t="s">
+      <c r="A66" s="50" t="s">
         <v>538</v>
       </c>
-      <c r="B66" s="84">
+      <c r="B66" s="49">
         <f>B48</f>
         <v>1.68</v>
       </c>
-      <c r="C66" s="84">
+      <c r="C66" s="49">
         <f>C48</f>
         <v>0.32</v>
       </c>
-      <c r="D66" s="84">
+      <c r="D66" s="49">
         <f>AVERAGE(A60)</f>
         <v>6.1813186813186816E-2</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="87"/>
-      <c r="B71" s="84" t="s">
+      <c r="A71" s="52"/>
+      <c r="B71" s="49" t="s">
         <v>512</v>
       </c>
-      <c r="C71" s="84" t="s">
+      <c r="C71" s="49" t="s">
         <v>513</v>
       </c>
-      <c r="D71" s="84" t="s">
+      <c r="D71" s="49" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="85" t="s">
+      <c r="A72" s="50" t="s">
         <v>510</v>
       </c>
-      <c r="B72" s="84">
+      <c r="B72" s="49">
         <v>1.68</v>
       </c>
-      <c r="C72" s="84">
+      <c r="C72" s="49">
         <v>0.32</v>
       </c>
-      <c r="D72" s="84">
+      <c r="D72" s="49">
         <v>6.758352432406016E-2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="85" t="s">
+      <c r="A73" s="50" t="s">
         <v>511</v>
       </c>
-      <c r="B73" s="84">
+      <c r="B73" s="49">
         <v>1.68</v>
       </c>
-      <c r="C73" s="84">
+      <c r="C73" s="49">
         <v>0.32</v>
       </c>
-      <c r="D73" s="84">
+      <c r="D73" s="49">
         <v>1.3368169646517398E-2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="88" t="s">
+      <c r="A74" s="53" t="s">
         <v>537</v>
       </c>
-      <c r="B74" s="86">
+      <c r="B74" s="51">
         <v>1.68</v>
       </c>
-      <c r="C74" s="86">
+      <c r="C74" s="51">
         <v>0.32</v>
       </c>
-      <c r="D74" s="86">
+      <c r="D74" s="51">
         <v>0.3125</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="88" t="s">
+      <c r="A75" s="53" t="s">
         <v>538</v>
       </c>
-      <c r="B75" s="86">
+      <c r="B75" s="51">
         <v>1.68</v>
       </c>
-      <c r="C75" s="86">
+      <c r="C75" s="51">
         <v>0.32</v>
       </c>
-      <c r="D75" s="86">
+      <c r="D75" s="51">
         <v>6.1813186813186816E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A19:I19"/>
     <mergeCell ref="A39:I39"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="A52:J52"/>
     <mergeCell ref="A54:I54"/>
     <mergeCell ref="C57:C58"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A19:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68D1AFF-A559-F545-B121-69B0DF3FAC36}">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="90" t="s">
+        <v>540</v>
+      </c>
+      <c r="B3" s="87" t="s">
+        <v>541</v>
+      </c>
+      <c r="C3" s="90" t="s">
+        <v>627</v>
+      </c>
+      <c r="D3" s="90" t="s">
+        <v>543</v>
+      </c>
+      <c r="E3" s="90" t="s">
+        <v>544</v>
+      </c>
+      <c r="F3" s="90" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="90"/>
+      <c r="B4" s="27" t="s">
+        <v>542</v>
+      </c>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="J4" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
+        <v>546</v>
+      </c>
+      <c r="B5" s="89">
+        <v>391.4</v>
+      </c>
+      <c r="C5" s="89" t="s">
+        <v>547</v>
+      </c>
+      <c r="D5" s="89" t="s">
+        <v>548</v>
+      </c>
+      <c r="E5" s="89" t="s">
+        <v>549</v>
+      </c>
+      <c r="F5" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H5" t="str" cm="1">
+        <f t="array" ref="H5:I5">_xlfn.TEXTSPLIT(C5,"kg")</f>
+        <v>48,000 </v>
+      </c>
+      <c r="I5" t="str">
+        <v xml:space="preserve"> (106,000 lb)</v>
+      </c>
+      <c r="J5" s="3">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>551</v>
+      </c>
+      <c r="B6" s="89">
+        <v>475</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>552</v>
+      </c>
+      <c r="D6" s="89" t="s">
+        <v>553</v>
+      </c>
+      <c r="E6" s="89" t="s">
+        <v>549</v>
+      </c>
+      <c r="F6" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H6" t="str" cm="1">
+        <f t="array" ref="H6:I6">_xlfn.TEXTSPLIT(C6,"kg")</f>
+        <v>70,000 </v>
+      </c>
+      <c r="I6" t="str">
+        <v xml:space="preserve"> (154,000 lb)</v>
+      </c>
+      <c r="J6">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="88" t="s">
+        <v>554</v>
+      </c>
+      <c r="B7" s="89">
+        <v>342</v>
+      </c>
+      <c r="C7" s="89" t="s">
+        <v>555</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>553</v>
+      </c>
+      <c r="E7" s="89" t="s">
+        <v>556</v>
+      </c>
+      <c r="F7" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H7" t="str" cm="1">
+        <f t="array" ref="H7:I7">_xlfn.TEXTSPLIT(C7,"kg")</f>
+        <v>68,000 </v>
+      </c>
+      <c r="I7" t="str">
+        <v xml:space="preserve"> (150,000 lb)</v>
+      </c>
+      <c r="J7">
+        <v>68000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="27" t="s">
+        <v>557</v>
+      </c>
+      <c r="B8" s="89">
+        <v>270</v>
+      </c>
+      <c r="C8" s="89" t="s">
+        <v>558</v>
+      </c>
+      <c r="D8" s="89" t="s">
+        <v>559</v>
+      </c>
+      <c r="E8" s="89" t="s">
+        <v>560</v>
+      </c>
+      <c r="F8" s="89" t="s">
+        <v>561</v>
+      </c>
+      <c r="H8" t="str" cm="1">
+        <f t="array" ref="H8:I8">_xlfn.TEXTSPLIT(C8,"kg")</f>
+        <v>37,000 </v>
+      </c>
+      <c r="I8" t="str">
+        <v xml:space="preserve"> (82,000 lb)</v>
+      </c>
+      <c r="J8">
+        <v>37000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="27" t="s">
+        <v>562</v>
+      </c>
+      <c r="B9" s="89">
+        <v>1210</v>
+      </c>
+      <c r="C9" s="89" t="s">
+        <v>563</v>
+      </c>
+      <c r="D9" s="89" t="s">
+        <v>548</v>
+      </c>
+      <c r="E9" s="89" t="s">
+        <v>564</v>
+      </c>
+      <c r="F9" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H9" t="str" cm="1">
+        <f t="array" ref="H9:I9">_xlfn.TEXTSPLIT(C9,"kg")</f>
+        <v>47,000 </v>
+      </c>
+      <c r="I9" t="str">
+        <v xml:space="preserve"> (104,000 lb)</v>
+      </c>
+      <c r="J9">
+        <v>47000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="27" t="s">
+        <v>565</v>
+      </c>
+      <c r="B10" s="89">
+        <v>2615</v>
+      </c>
+      <c r="C10" s="89" t="s">
+        <v>566</v>
+      </c>
+      <c r="D10" s="89" t="s">
+        <v>548</v>
+      </c>
+      <c r="E10" s="89" t="s">
+        <v>567</v>
+      </c>
+      <c r="F10" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H10" t="str" cm="1">
+        <f t="array" ref="H10:I10">_xlfn.TEXTSPLIT(C10,"kg")</f>
+        <v>53,000 </v>
+      </c>
+      <c r="I10" t="str">
+        <v xml:space="preserve"> (117,000 lb)</v>
+      </c>
+      <c r="J10">
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
+        <v>568</v>
+      </c>
+      <c r="B11" s="89">
+        <v>639</v>
+      </c>
+      <c r="C11" s="89" t="s">
+        <v>569</v>
+      </c>
+      <c r="D11" s="89" t="s">
+        <v>570</v>
+      </c>
+      <c r="E11" s="89" t="s">
+        <v>571</v>
+      </c>
+      <c r="F11" s="89" t="s">
+        <v>572</v>
+      </c>
+      <c r="H11" t="str" cm="1">
+        <f t="array" ref="H11:I11">_xlfn.TEXTSPLIT(C11,"kg")</f>
+        <v>80,000 </v>
+      </c>
+      <c r="I11" t="str">
+        <v xml:space="preserve"> (176,000 lb)</v>
+      </c>
+      <c r="J11">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="27" t="s">
+        <v>573</v>
+      </c>
+      <c r="B12" s="89">
+        <v>1028</v>
+      </c>
+      <c r="C12" s="89" t="s">
+        <v>574</v>
+      </c>
+      <c r="D12" s="89" t="s">
+        <v>575</v>
+      </c>
+      <c r="E12" s="89" t="s">
+        <v>576</v>
+      </c>
+      <c r="F12" s="89" t="s">
+        <v>572</v>
+      </c>
+      <c r="H12" t="str" cm="1">
+        <f t="array" ref="H12:I12">_xlfn.TEXTSPLIT(C12,"kg")</f>
+        <v>150,000 </v>
+      </c>
+      <c r="I12" t="str">
+        <v xml:space="preserve"> (331,000 lb)</v>
+      </c>
+      <c r="J12">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="27" t="s">
+        <v>577</v>
+      </c>
+      <c r="B13" s="89">
+        <v>1300</v>
+      </c>
+      <c r="C13" s="89" t="s">
+        <v>578</v>
+      </c>
+      <c r="D13" s="89" t="s">
+        <v>575</v>
+      </c>
+      <c r="E13" s="89" t="s">
+        <v>579</v>
+      </c>
+      <c r="F13" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H13" t="str" cm="1">
+        <f t="array" ref="H13:I13">_xlfn.TEXTSPLIT(C13,"kg")</f>
+        <v>250,000 </v>
+      </c>
+      <c r="I13" t="str">
+        <v xml:space="preserve"> (551,000 lb)</v>
+      </c>
+      <c r="J13">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="27" t="s">
+        <v>580</v>
+      </c>
+      <c r="B14" s="89">
+        <v>107.6</v>
+      </c>
+      <c r="C14" s="89" t="s">
+        <v>581</v>
+      </c>
+      <c r="D14" s="89" t="s">
+        <v>582</v>
+      </c>
+      <c r="E14" s="89" t="s">
+        <v>583</v>
+      </c>
+      <c r="F14" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H14" t="str" cm="1">
+        <f t="array" ref="H14:I14">_xlfn.TEXTSPLIT(C14,"kg")</f>
+        <v>18,200 </v>
+      </c>
+      <c r="I14" t="str">
+        <v xml:space="preserve"> (40,000 lb)</v>
+      </c>
+      <c r="J14">
+        <v>18200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="27" t="s">
+        <v>584</v>
+      </c>
+      <c r="B15" s="89">
+        <v>1840</v>
+      </c>
+      <c r="C15" s="89" t="s">
+        <v>585</v>
+      </c>
+      <c r="D15" s="89" t="s">
+        <v>586</v>
+      </c>
+      <c r="E15" s="89" t="s">
+        <v>587</v>
+      </c>
+      <c r="F15" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H15" t="str" cm="1">
+        <f t="array" ref="H15:I15">_xlfn.TEXTSPLIT(C15,"kg")</f>
+        <v>83,325 </v>
+      </c>
+      <c r="I15" t="str">
+        <v xml:space="preserve"> (183,700 lb)</v>
+      </c>
+      <c r="J15">
+        <v>83325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="27" t="s">
+        <v>588</v>
+      </c>
+      <c r="B16" s="89">
+        <v>854.5</v>
+      </c>
+      <c r="C16" s="89" t="s">
+        <v>589</v>
+      </c>
+      <c r="D16" s="89" t="s">
+        <v>590</v>
+      </c>
+      <c r="E16" s="89" t="s">
+        <v>591</v>
+      </c>
+      <c r="F16" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H16" t="str" cm="1">
+        <f t="array" ref="H16:I16">_xlfn.TEXTSPLIT(C16,"kg")</f>
+        <v>134,200 </v>
+      </c>
+      <c r="I16" t="str">
+        <v xml:space="preserve"> (295,900 lb)</v>
+      </c>
+      <c r="J16">
+        <v>134200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="27" t="s">
+        <v>592</v>
+      </c>
+      <c r="B17" s="89">
+        <v>239</v>
+      </c>
+      <c r="C17" s="89" t="s">
+        <v>593</v>
+      </c>
+      <c r="D17" s="89" t="s">
+        <v>594</v>
+      </c>
+      <c r="E17" s="89" t="s">
+        <v>595</v>
+      </c>
+      <c r="F17" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H17" t="str" cm="1">
+        <f t="array" ref="H17:I17">_xlfn.TEXTSPLIT(C17,"kg")</f>
+        <v>39,780 </v>
+      </c>
+      <c r="I17" t="str">
+        <v xml:space="preserve"> (87,700 lb)</v>
+      </c>
+      <c r="J17">
+        <v>39780</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="27" t="s">
+        <v>596</v>
+      </c>
+      <c r="B18" s="89">
+        <v>438.2</v>
+      </c>
+      <c r="C18" s="89" t="s">
+        <v>597</v>
+      </c>
+      <c r="D18" s="89" t="s">
+        <v>598</v>
+      </c>
+      <c r="E18" s="89" t="s">
+        <v>599</v>
+      </c>
+      <c r="F18" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H18" t="str" cm="1">
+        <f t="array" ref="H18:I18">_xlfn.TEXTSPLIT(C18,"kg")</f>
+        <v>52,700 </v>
+      </c>
+      <c r="I18" t="str">
+        <v xml:space="preserve"> (116,200 lb)</v>
+      </c>
+      <c r="J18">
+        <v>52700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
+        <v>600</v>
+      </c>
+      <c r="B19" s="89">
+        <v>653</v>
+      </c>
+      <c r="C19" s="89" t="s">
+        <v>601</v>
+      </c>
+      <c r="D19" s="89" t="s">
+        <v>602</v>
+      </c>
+      <c r="E19" s="89" t="s">
+        <v>603</v>
+      </c>
+      <c r="F19" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H19" t="str" cm="1">
+        <f t="array" ref="H19:I19">_xlfn.TEXTSPLIT(C19,"kg")</f>
+        <v>103,000 </v>
+      </c>
+      <c r="I19" t="str">
+        <v xml:space="preserve"> (227,000 lb)</v>
+      </c>
+      <c r="J19">
+        <v>103000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
+        <v>604</v>
+      </c>
+      <c r="B20" s="89"/>
+      <c r="C20" s="89" t="s">
+        <v>605</v>
+      </c>
+      <c r="D20" s="89" t="s">
+        <v>606</v>
+      </c>
+      <c r="E20" s="89" t="s">
+        <v>607</v>
+      </c>
+      <c r="F20" s="89" t="s">
+        <v>561</v>
+      </c>
+      <c r="H20" t="str" cm="1">
+        <f t="array" ref="H20:I20">_xlfn.TEXTSPLIT(C20,"kg")</f>
+        <v>77,519 </v>
+      </c>
+      <c r="I20" t="str">
+        <v xml:space="preserve"> (170,900 lb)</v>
+      </c>
+      <c r="J20">
+        <v>77519</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="27" t="s">
+        <v>608</v>
+      </c>
+      <c r="B21" s="89">
+        <v>39</v>
+      </c>
+      <c r="C21" s="89" t="s">
+        <v>609</v>
+      </c>
+      <c r="D21" s="89" t="s">
+        <v>610</v>
+      </c>
+      <c r="E21" s="89" t="s">
+        <v>611</v>
+      </c>
+      <c r="F21" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H21" t="str" cm="1">
+        <f t="array" ref="H21:I21">_xlfn.TEXTSPLIT(C21,"kg")</f>
+        <v>4,700 </v>
+      </c>
+      <c r="I21" t="str">
+        <v xml:space="preserve"> (10,400 lb)</v>
+      </c>
+      <c r="J21">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="27" t="s">
+        <v>612</v>
+      </c>
+      <c r="B22" s="89"/>
+      <c r="C22" s="89" t="s">
+        <v>613</v>
+      </c>
+      <c r="D22" s="89" t="s">
+        <v>590</v>
+      </c>
+      <c r="E22" s="89" t="s">
+        <v>614</v>
+      </c>
+      <c r="F22" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H22" t="str" cm="1">
+        <f t="array" ref="H22:I22">_xlfn.TEXTSPLIT(C22,"kg")</f>
+        <v>77,000 </v>
+      </c>
+      <c r="I22" t="str">
+        <v xml:space="preserve"> (170,000 lb)</v>
+      </c>
+      <c r="J22">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="27" t="s">
+        <v>615</v>
+      </c>
+      <c r="B23" s="89"/>
+      <c r="C23" s="89" t="s">
+        <v>616</v>
+      </c>
+      <c r="D23" s="89" t="s">
+        <v>617</v>
+      </c>
+      <c r="E23" s="89" t="s">
+        <v>618</v>
+      </c>
+      <c r="F23" s="89" t="s">
+        <v>561</v>
+      </c>
+      <c r="H23" t="str" cm="1">
+        <f t="array" ref="H23:I23">_xlfn.TEXTSPLIT(C23,"kg")</f>
+        <v>122,470 </v>
+      </c>
+      <c r="I23" t="str">
+        <v xml:space="preserve"> (270,000 lb)</v>
+      </c>
+      <c r="J23">
+        <v>122470</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="27" t="s">
+        <v>619</v>
+      </c>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89" t="s">
+        <v>620</v>
+      </c>
+      <c r="D24" s="89" t="s">
+        <v>621</v>
+      </c>
+      <c r="E24" s="89" t="s">
+        <v>622</v>
+      </c>
+      <c r="F24" s="89" t="s">
+        <v>561</v>
+      </c>
+      <c r="H24" t="str" cm="1">
+        <f t="array" ref="H24:I24">_xlfn.TEXTSPLIT(C24,"kg")</f>
+        <v>20,400 </v>
+      </c>
+      <c r="I24" t="str">
+        <v xml:space="preserve"> (45,000 lb)</v>
+      </c>
+      <c r="J24">
+        <v>20400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="27" t="s">
+        <v>623</v>
+      </c>
+      <c r="B25" s="89">
+        <v>440</v>
+      </c>
+      <c r="C25" s="89" t="s">
+        <v>624</v>
+      </c>
+      <c r="D25" s="89" t="s">
+        <v>625</v>
+      </c>
+      <c r="E25" s="89" t="s">
+        <v>626</v>
+      </c>
+      <c r="F25" s="89" t="s">
+        <v>550</v>
+      </c>
+      <c r="H25" t="str" cm="1">
+        <f t="array" ref="H25:I25">_xlfn.TEXTSPLIT(C25,"kg")</f>
+        <v>91,670 </v>
+      </c>
+      <c r="I25" t="str">
+        <v xml:space="preserve"> (202,100 lb)</v>
+      </c>
+      <c r="J25">
+        <v>91670</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J26" s="3">
+        <f>AVERAGE(J5:J25)</f>
+        <v>77522.095238095237</v>
+      </c>
+      <c r="K26" s="91">
+        <f>MEDIAN(J5:J25)</f>
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>295</v>
+      </c>
+      <c r="K27" t="s">
+        <v>630</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" tooltip="Cubic metre" display="https://en.wikipedia.org/wiki/Cubic_metre" xr:uid="{716BB53A-8A82-E243-B070-B4BDD5A6B3E9}"/>
+    <hyperlink ref="A5" r:id="rId2" tooltip="Airbus A300" display="https://en.wikipedia.org/wiki/Airbus_A300" xr:uid="{95F26463-B9D5-7F4A-8594-F6B9113312A3}"/>
+    <hyperlink ref="A6" r:id="rId3" tooltip="Airbus A330" display="https://en.wikipedia.org/wiki/Airbus_A330" xr:uid="{6870B1AB-9383-1B43-AA7A-B31D20889EA0}"/>
+    <hyperlink ref="A8" r:id="rId4" tooltip="Airbus A400M" display="https://en.wikipedia.org/wiki/Airbus_A400M" xr:uid="{27403542-A650-1B4C-BECC-A346A511746D}"/>
+    <hyperlink ref="A9" r:id="rId5" tooltip="Airbus Beluga" display="https://en.wikipedia.org/wiki/Airbus_Beluga" xr:uid="{329D1E4B-4234-6948-92D5-A62E6BF89282}"/>
+    <hyperlink ref="A10" r:id="rId6" tooltip="Airbus BelugaXL" display="https://en.wikipedia.org/wiki/Airbus_BelugaXL" xr:uid="{44CB45C1-52D9-4F47-910F-B2B758F5227C}"/>
+    <hyperlink ref="A11" r:id="rId7" tooltip="Antonov An-22" display="https://en.wikipedia.org/wiki/Antonov_An-22" xr:uid="{5A4A0333-67B3-5246-A1F5-D87C77D2D48E}"/>
+    <hyperlink ref="A12" r:id="rId8" tooltip="Antonov An-124" display="https://en.wikipedia.org/wiki/Antonov_An-124" xr:uid="{7DBEB74A-968C-ED4C-A539-37B842019D34}"/>
+    <hyperlink ref="A13" r:id="rId9" tooltip="Antonov An-225" display="https://en.wikipedia.org/wiki/Antonov_An-225" xr:uid="{BD807389-7DBD-0D40-A042-5E84651FBB87}"/>
+    <hyperlink ref="A14" r:id="rId10" tooltip="Boeing 737" display="https://en.wikipedia.org/wiki/Boeing_737" xr:uid="{CA9BD140-535B-A849-8538-5332020E5DED}"/>
+    <hyperlink ref="A15" r:id="rId11" tooltip="Boeing 747 LCF" display="https://en.wikipedia.org/wiki/Boeing_747_LCF" xr:uid="{8E0605BF-2835-D348-A95F-FB56CD863763}"/>
+    <hyperlink ref="A16" r:id="rId12" tooltip="Boeing 747-8F" display="https://en.wikipedia.org/wiki/Boeing_747-8F" xr:uid="{850603C3-14C6-984B-87FE-0BC6C9874D35}"/>
+    <hyperlink ref="A17" r:id="rId13" tooltip="Boeing 757" display="https://en.wikipedia.org/wiki/Boeing_757" xr:uid="{DB90FC72-0D03-224D-8433-C245858C284B}"/>
+    <hyperlink ref="A18" r:id="rId14" tooltip="Boeing 767" display="https://en.wikipedia.org/wiki/Boeing_767" xr:uid="{D39EB07D-4E45-A349-82DE-91EC8918EC51}"/>
+    <hyperlink ref="A19" r:id="rId15" tooltip="Boeing 777" display="https://en.wikipedia.org/wiki/Boeing_777" xr:uid="{E7C4B320-EEEE-1148-B876-ABEA6EA2C555}"/>
+    <hyperlink ref="A20" r:id="rId16" tooltip="Boeing C-17" display="https://en.wikipedia.org/wiki/Boeing_C-17" xr:uid="{2E8DE230-B6D6-554E-A645-F6FA4F4E476E}"/>
+    <hyperlink ref="A21" r:id="rId17" tooltip="Bombardier Dash 8" display="https://en.wikipedia.org/wiki/Bombardier_Dash_8" xr:uid="{8F623ED3-67C7-DF47-9368-209A274ABC48}"/>
+    <hyperlink ref="A22" r:id="rId18" tooltip="Douglas DC-10" display="https://en.wikipedia.org/wiki/Douglas_DC-10" xr:uid="{74C40AA7-8C82-FC49-BDF9-69AD7E97F3C3}"/>
+    <hyperlink ref="A23" r:id="rId19" tooltip="Lockheed C-5" display="https://en.wikipedia.org/wiki/Lockheed_C-5" xr:uid="{275E6E3F-1CFE-E24D-8F02-EA7CAC0F489B}"/>
+    <hyperlink ref="A24" r:id="rId20" tooltip="Lockheed C-130" display="https://en.wikipedia.org/wiki/Lockheed_C-130" xr:uid="{79FE279A-D61F-3749-95CF-8C7BE7F79D34}"/>
+    <hyperlink ref="A25" r:id="rId21" tooltip="McDonnell Douglas MD-11" display="https://en.wikipedia.org/wiki/McDonnell_Douglas_MD-11" xr:uid="{C91F0480-FC3B-3245-8865-CA741FF18F93}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201F496F-0260-FD4C-850F-564E18865F2A}">
   <dimension ref="A9:O32"/>
   <sheetViews>
@@ -4754,43 +5822,43 @@
   </cols>
   <sheetData>
     <row r="9" spans="1:10" ht="26" x14ac:dyDescent="0.3">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="85" t="s">
         <v>514</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-    </row>
-    <row r="10" spans="1:10" s="80" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+    </row>
+    <row r="10" spans="1:10" ht="26" x14ac:dyDescent="0.3">
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
     </row>
     <row r="11" spans="1:10" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="83" t="s">
         <v>515</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -4832,11 +5900,11 @@
       <c r="D18" t="s">
         <v>523</v>
       </c>
-      <c r="M18" s="65" t="s">
+      <c r="M18" s="56" t="s">
         <v>521</v>
       </c>
-      <c r="N18" s="65"/>
-      <c r="O18" s="65"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="56"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C19">
@@ -4848,9 +5916,9 @@
       <c r="E19" t="s">
         <v>524</v>
       </c>
-      <c r="M19" s="65"/>
-      <c r="N19" s="65"/>
-      <c r="O19" s="65"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="56"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C20">
@@ -4862,9 +5930,9 @@
       <c r="E20" t="s">
         <v>525</v>
       </c>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="65"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="56"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C21">
@@ -4891,7 +5959,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="C25" s="83">
+      <c r="C25" s="48">
         <v>-7.0092399999999999E-3</v>
       </c>
       <c r="D25">
@@ -5078,19 +6146,19 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="62"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
       <c r="L11" t="s">
         <v>90</v>
       </c>
@@ -5114,42 +6182,42 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="174" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="56"/>
-      <c r="P15" s="56"/>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="56"/>
-      <c r="U15" s="56"/>
-      <c r="V15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
+      <c r="U15" s="57"/>
+      <c r="V15" s="57"/>
     </row>
     <row r="16" spans="1:22" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
-      <c r="R16" s="57"/>
-      <c r="S16" s="57"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="62"/>
+      <c r="P16" s="62"/>
+      <c r="Q16" s="62"/>
+      <c r="R16" s="62"/>
+      <c r="S16" s="62"/>
       <c r="T16" s="18"/>
       <c r="U16" s="18"/>
     </row>
@@ -5196,7 +6264,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="59" t="s">
         <v>88</v>
       </c>
       <c r="B18" t="s">
@@ -5250,7 +6318,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="53"/>
+      <c r="A19" s="59"/>
       <c r="B19" t="s">
         <v>36</v>
       </c>
@@ -5302,7 +6370,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="53"/>
+      <c r="A20" s="59"/>
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -5354,7 +6422,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21" s="53"/>
+      <c r="A21" s="59"/>
       <c r="B21" s="8" t="s">
         <v>85</v>
       </c>
@@ -5403,7 +6471,7 @@
       <c r="S21" s="8"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A22" s="53"/>
+      <c r="A22" s="59"/>
       <c r="B22" s="8" t="s">
         <v>86</v>
       </c>
@@ -5434,7 +6502,7 @@
       <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A23" s="53"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="8" t="s">
         <v>87</v>
       </c>
@@ -5466,7 +6534,7 @@
       <c r="S23" s="8"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="53"/>
+      <c r="A24" s="59"/>
       <c r="B24" t="s">
         <v>39</v>
       </c>
@@ -5490,7 +6558,7 @@
       <c r="A25" s="20"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="59" t="s">
         <v>89</v>
       </c>
       <c r="B26" t="s">
@@ -5513,7 +6581,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A27" s="53"/>
+      <c r="A27" s="59"/>
       <c r="B27" t="s">
         <v>91</v>
       </c>
@@ -5540,10 +6608,10 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C28" s="8"/>
-      <c r="N28" s="61"/>
-      <c r="O28" s="61"/>
-      <c r="P28" s="61"/>
-      <c r="Q28" s="61"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="58"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="58"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C29" s="8"/>
@@ -5561,14 +6629,14 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J30" s="63" t="s">
+      <c r="J30" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="K30" s="50" t="s">
+      <c r="K30" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="L30" s="51"/>
-      <c r="M30" s="58"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="65"/>
       <c r="N30" s="9">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -5583,12 +6651,12 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J31" s="63"/>
-      <c r="K31" s="52" t="s">
+      <c r="J31" s="61"/>
+      <c r="K31" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="L31" s="53"/>
-      <c r="M31" s="59"/>
+      <c r="L31" s="59"/>
+      <c r="M31" s="67"/>
       <c r="N31" s="12">
         <v>0.83</v>
       </c>
@@ -5607,12 +6675,12 @@
         <f>(0.0022*0.037)^0.5</f>
         <v>9.0221948549119683E-3</v>
       </c>
-      <c r="J32" s="63"/>
-      <c r="K32" s="54" t="s">
+      <c r="J32" s="61"/>
+      <c r="K32" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="L32" s="55"/>
-      <c r="M32" s="60"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="70"/>
       <c r="N32" s="14">
         <v>0.1</v>
       </c>
@@ -5627,14 +6695,14 @@
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J33" s="49" t="s">
+      <c r="J33" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="K33" s="50" t="s">
+      <c r="K33" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="L33" s="51"/>
-      <c r="M33" s="58"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="65"/>
       <c r="N33" s="9">
         <v>0.09</v>
       </c>
@@ -5649,12 +6717,12 @@
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J34" s="49"/>
-      <c r="K34" s="52" t="s">
+      <c r="J34" s="60"/>
+      <c r="K34" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="L34" s="53"/>
-      <c r="M34" s="59"/>
+      <c r="L34" s="59"/>
+      <c r="M34" s="67"/>
       <c r="N34" s="12">
         <v>0.78</v>
       </c>
@@ -5669,12 +6737,12 @@
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J35" s="49"/>
-      <c r="K35" s="54" t="s">
+      <c r="J35" s="60"/>
+      <c r="K35" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="L35" s="55"/>
-      <c r="M35" s="60"/>
+      <c r="L35" s="69"/>
+      <c r="M35" s="70"/>
       <c r="N35" s="14">
         <v>0.13</v>
       </c>
@@ -5689,14 +6757,14 @@
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J36" s="49" t="s">
+      <c r="J36" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="K36" s="50" t="s">
+      <c r="K36" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="L36" s="51"/>
-      <c r="M36" s="58"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="65"/>
       <c r="N36" s="9">
         <v>0.2</v>
       </c>
@@ -5711,12 +6779,12 @@
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J37" s="49"/>
-      <c r="K37" s="52" t="s">
+      <c r="J37" s="60"/>
+      <c r="K37" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="L37" s="53"/>
-      <c r="M37" s="59"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="67"/>
       <c r="N37" s="12">
         <v>0.8</v>
       </c>
@@ -5731,12 +6799,12 @@
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J38" s="49"/>
-      <c r="K38" s="54" t="s">
+      <c r="J38" s="60"/>
+      <c r="K38" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="L38" s="55"/>
-      <c r="M38" s="60"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="70"/>
       <c r="N38" s="12">
         <v>0</v>
       </c>
@@ -5751,14 +6819,14 @@
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J39" s="49" t="s">
+      <c r="J39" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="K39" s="50" t="s">
+      <c r="K39" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="L39" s="51"/>
-      <c r="M39" s="51"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="64"/>
       <c r="N39" s="9">
         <f>AVERAGE(N30,N33,N36)</f>
         <v>0.12</v>
@@ -5777,12 +6845,12 @@
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J40" s="49"/>
-      <c r="K40" s="52" t="s">
+      <c r="J40" s="60"/>
+      <c r="K40" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="L40" s="53"/>
-      <c r="M40" s="53"/>
+      <c r="L40" s="59"/>
+      <c r="M40" s="59"/>
       <c r="N40" s="12">
         <f t="shared" ref="N40:Q41" si="5">AVERAGE(N31,N34,N37)</f>
         <v>0.80333333333333334</v>
@@ -5801,12 +6869,12 @@
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J41" s="49"/>
-      <c r="K41" s="54" t="s">
+      <c r="J41" s="60"/>
+      <c r="K41" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="L41" s="55"/>
-      <c r="M41" s="55"/>
+      <c r="L41" s="69"/>
+      <c r="M41" s="69"/>
       <c r="N41" s="14">
         <f t="shared" si="5"/>
         <v>7.6666666666666675E-2</v>
@@ -5853,14 +6921,14 @@
       <c r="G43" t="s">
         <v>47</v>
       </c>
-      <c r="I43" s="48" t="s">
+      <c r="I43" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="J43" s="48"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="47">
+      <c r="J43" s="72"/>
+      <c r="K43" s="72"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="72"/>
+      <c r="N43" s="71">
         <f>1-N42</f>
         <v>8.7121212121212155E-2</v>
       </c>
@@ -5885,12 +6953,12 @@
         <f>F43-F22-F23</f>
         <v>6.8000000000000027E-8</v>
       </c>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="48"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="47"/>
+      <c r="I44" s="72"/>
+      <c r="J44" s="72"/>
+      <c r="K44" s="72"/>
+      <c r="L44" s="72"/>
+      <c r="M44" s="72"/>
+      <c r="N44" s="71"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
@@ -6007,19 +7075,19 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="62" t="s">
+      <c r="A51" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="B51" s="62"/>
-      <c r="C51" s="62"/>
-      <c r="D51" s="62"/>
-      <c r="E51" s="62"/>
-      <c r="F51" s="62"/>
-      <c r="G51" s="62"/>
-      <c r="H51" s="62"/>
-      <c r="I51" s="62"/>
-      <c r="J51" s="62"/>
-      <c r="K51" s="62"/>
+      <c r="B51" s="54"/>
+      <c r="C51" s="54"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="54"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="54"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="54"/>
+      <c r="K51" s="54"/>
     </row>
     <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="26" t="s">
@@ -6038,19 +7106,19 @@
     </row>
     <row r="56" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="62" t="s">
+      <c r="A57" s="54" t="s">
         <v>144</v>
       </c>
-      <c r="B57" s="62"/>
-      <c r="C57" s="62"/>
-      <c r="D57" s="62"/>
-      <c r="E57" s="62"/>
-      <c r="F57" s="62"/>
-      <c r="G57" s="62"/>
-      <c r="H57" s="62"/>
-      <c r="I57" s="62"/>
-      <c r="J57" s="62"/>
-      <c r="K57" s="62"/>
+      <c r="B57" s="54"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="54"/>
+      <c r="G57" s="54"/>
+      <c r="H57" s="54"/>
+      <c r="I57" s="54"/>
+      <c r="J57" s="54"/>
+      <c r="K57" s="54"/>
     </row>
     <row r="58" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="26" t="s">
@@ -6076,34 +7144,34 @@
       </c>
     </row>
     <row r="64" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A64" s="62" t="s">
+      <c r="A64" s="54" t="s">
         <v>280</v>
       </c>
-      <c r="B64" s="62"/>
-      <c r="C64" s="62"/>
-      <c r="D64" s="62"/>
-      <c r="E64" s="62"/>
-      <c r="F64" s="62"/>
-      <c r="G64" s="62"/>
-      <c r="H64" s="62"/>
-      <c r="I64" s="62"/>
-      <c r="J64" s="62"/>
-      <c r="K64" s="62"/>
+      <c r="B64" s="54"/>
+      <c r="C64" s="54"/>
+      <c r="D64" s="54"/>
+      <c r="E64" s="54"/>
+      <c r="F64" s="54"/>
+      <c r="G64" s="54"/>
+      <c r="H64" s="54"/>
+      <c r="I64" s="54"/>
+      <c r="J64" s="54"/>
+      <c r="K64" s="54"/>
     </row>
     <row r="71" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A71" s="62" t="s">
+      <c r="A71" s="54" t="s">
         <v>315</v>
       </c>
-      <c r="B71" s="62"/>
-      <c r="C71" s="62"/>
-      <c r="D71" s="62"/>
-      <c r="E71" s="62"/>
-      <c r="F71" s="62"/>
-      <c r="G71" s="62"/>
-      <c r="H71" s="62"/>
-      <c r="I71" s="62"/>
-      <c r="J71" s="62"/>
-      <c r="K71" s="62"/>
+      <c r="B71" s="54"/>
+      <c r="C71" s="54"/>
+      <c r="D71" s="54"/>
+      <c r="E71" s="54"/>
+      <c r="F71" s="54"/>
+      <c r="G71" s="54"/>
+      <c r="H71" s="54"/>
+      <c r="I71" s="54"/>
+      <c r="J71" s="54"/>
+      <c r="K71" s="54"/>
     </row>
     <row r="72" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="26" t="s">
@@ -6116,10 +7184,10 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="64" t="s">
+      <c r="A74" s="55" t="s">
         <v>309</v>
       </c>
-      <c r="B74" s="64"/>
+      <c r="B74" s="55"/>
       <c r="C74" s="42" t="s">
         <v>109</v>
       </c>
@@ -6144,10 +7212,10 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" s="64" t="s">
+      <c r="A76" s="55" t="s">
         <v>317</v>
       </c>
-      <c r="B76" s="64"/>
+      <c r="B76" s="55"/>
       <c r="C76" s="41">
         <f>C75*$B$80</f>
         <v>2.6086956521739112E-4</v>
@@ -6218,21 +7286,12 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A71:K71"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="A64:K64"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="J36:J38"/>
-    <mergeCell ref="J33:J35"/>
-    <mergeCell ref="J30:J32"/>
+    <mergeCell ref="N43:N44"/>
+    <mergeCell ref="I43:M44"/>
+    <mergeCell ref="J39:J41"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="K41:M41"/>
     <mergeCell ref="N15:V15"/>
     <mergeCell ref="R16:S16"/>
     <mergeCell ref="K36:M36"/>
@@ -6246,12 +7305,21 @@
     <mergeCell ref="N28:Q28"/>
     <mergeCell ref="K34:M34"/>
     <mergeCell ref="K35:M35"/>
-    <mergeCell ref="N43:N44"/>
-    <mergeCell ref="I43:M44"/>
-    <mergeCell ref="J39:J41"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="J36:J38"/>
+    <mergeCell ref="J33:J35"/>
+    <mergeCell ref="J30:J32"/>
+    <mergeCell ref="A71:K71"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="A64:K64"/>
+    <mergeCell ref="A57:K57"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A55" r:id="rId1" xr:uid="{939BE22A-9CE0-E745-AEFB-468D46C49282}"/>
@@ -6390,10 +7458,10 @@
         <f>intro!B8</f>
         <v>0.68020000000000003</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="74" t="s">
         <v>334</v>
       </c>
-      <c r="N1" s="67"/>
+      <c r="N1" s="74"/>
     </row>
     <row r="2" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -6423,11 +7491,11 @@
       <c r="I2">
         <v>36000</v>
       </c>
-      <c r="J2" s="66" t="s">
+      <c r="J2" s="73" t="s">
         <v>327</v>
       </c>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
       <c r="M2" s="44" t="s">
         <v>98</v>
       </c>
@@ -6450,16 +7518,16 @@
       <c r="E3">
         <v>947813394500</v>
       </c>
-      <c r="F3" s="66" t="s">
+      <c r="F3" s="73" t="s">
         <v>329</v>
       </c>
       <c r="G3">
         <f>I2/G2</f>
         <v>52925610.114672154</v>
       </c>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
       <c r="M3" s="44" t="s">
         <v>333</v>
       </c>
@@ -6483,16 +7551,16 @@
         <f>I4*I5</f>
         <v>45307145.619999997</v>
       </c>
-      <c r="F4" s="66"/>
+      <c r="F4" s="73"/>
       <c r="H4" t="s">
         <v>330</v>
       </c>
       <c r="I4">
         <v>2204.62</v>
       </c>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
       <c r="M4" s="44" t="s">
         <v>335</v>
       </c>
@@ -6502,45 +7570,45 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F5" s="66"/>
+      <c r="F5" s="73"/>
       <c r="H5" t="s">
         <v>331</v>
       </c>
       <c r="I5">
         <v>20551</v>
       </c>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
       <c r="M5" s="44"/>
       <c r="N5" s="44"/>
     </row>
     <row r="6" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
       <c r="L6" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
@@ -6570,7 +7638,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="59" t="s">
         <v>88</v>
       </c>
       <c r="B9" t="s">
@@ -6612,7 +7680,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="53"/>
+      <c r="A10" s="59"/>
       <c r="B10" t="s">
         <v>122</v>
       </c>
@@ -6656,7 +7724,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="53"/>
+      <c r="A11" s="59"/>
       <c r="B11" t="s">
         <v>123</v>
       </c>
@@ -6696,7 +7764,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="53"/>
+      <c r="A12" s="59"/>
       <c r="B12" t="s">
         <v>124</v>
       </c>
@@ -6740,7 +7808,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="53"/>
+      <c r="A13" s="59"/>
       <c r="B13" t="s">
         <v>125</v>
       </c>
@@ -6762,7 +7830,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="59" t="s">
         <v>89</v>
       </c>
       <c r="B14" t="s">
@@ -6800,7 +7868,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="53"/>
+      <c r="A15" s="59"/>
       <c r="B15" t="s">
         <v>129</v>
       </c>
@@ -6836,7 +7904,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="53"/>
+      <c r="A16" s="59"/>
       <c r="B16" t="s">
         <v>126</v>
       </c>
@@ -6872,7 +7940,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="53"/>
+      <c r="A17" s="59"/>
       <c r="B17" t="s">
         <v>127</v>
       </c>
@@ -6909,19 +7977,19 @@
     </row>
     <row r="18" spans="1:15" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="62" t="s">
+      <c r="A19" s="54" t="s">
         <v>303</v>
       </c>
-      <c r="B19" s="62"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="62"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
     </row>
     <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
@@ -7049,10 +8117,10 @@
       <c r="B34">
         <v>408.31599999999997</v>
       </c>
-      <c r="D34" s="64" t="s">
+      <c r="D34" s="55" t="s">
         <v>309</v>
       </c>
-      <c r="E34" s="64"/>
+      <c r="E34" s="55"/>
       <c r="F34" s="42" t="s">
         <v>109</v>
       </c>
@@ -7093,10 +8161,10 @@
         <f>B34/B35</f>
         <v>1.6789999588798881E-2</v>
       </c>
-      <c r="D36" s="64" t="s">
+      <c r="D36" s="55" t="s">
         <v>313</v>
       </c>
-      <c r="E36" s="64"/>
+      <c r="E36" s="55"/>
       <c r="F36" s="41">
         <f>F35*B36</f>
         <v>3.3579999177597762E-5</v>
@@ -7141,19 +8209,19 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="62" t="s">
+      <c r="A40" s="54" t="s">
         <v>144</v>
       </c>
-      <c r="B40" s="62"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="62"/>
-      <c r="E40" s="62"/>
-      <c r="F40" s="62"/>
-      <c r="G40" s="62"/>
-      <c r="H40" s="62"/>
-      <c r="I40" s="62"/>
-      <c r="J40" s="62"/>
-      <c r="K40" s="62"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="54"/>
+      <c r="J40" s="54"/>
+      <c r="K40" s="54"/>
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="26" t="s">
@@ -7397,34 +8465,34 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="62"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="G16" s="61" t="s">
+      <c r="G16" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
-      <c r="N16" s="61" t="s">
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="N16" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="O16" s="61"/>
-      <c r="P16" s="61"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="58"/>
       <c r="S16" s="23"/>
       <c r="T16" s="23"/>
       <c r="U16" s="23"/>
@@ -8029,19 +9097,19 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="62" t="s">
+      <c r="A34" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="62"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="54"/>
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="26"/>
@@ -8051,19 +9119,19 @@
     </row>
     <row r="39" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="62" t="s">
+      <c r="A40" s="54" t="s">
         <v>144</v>
       </c>
-      <c r="B40" s="62"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="62"/>
-      <c r="E40" s="62"/>
-      <c r="F40" s="62"/>
-      <c r="G40" s="62"/>
-      <c r="H40" s="62"/>
-      <c r="I40" s="62"/>
-      <c r="J40" s="62"/>
-      <c r="K40" s="62"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="54"/>
+      <c r="J40" s="54"/>
+      <c r="K40" s="54"/>
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="26"/>
@@ -8256,21 +9324,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
@@ -8371,7 +9439,7 @@
       <c r="D10" s="33"/>
       <c r="E10" s="33"/>
       <c r="F10" s="33"/>
-      <c r="G10" s="68" t="s">
+      <c r="G10" s="75" t="s">
         <v>185</v>
       </c>
       <c r="J10" t="s">
@@ -8391,7 +9459,7 @@
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
-      <c r="G11" s="68"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="28"/>
@@ -8406,7 +9474,7 @@
       <c r="D12" s="33"/>
       <c r="E12" s="33"/>
       <c r="F12" s="33"/>
-      <c r="G12" s="68"/>
+      <c r="G12" s="75"/>
       <c r="J12">
         <v>0.09</v>
       </c>
@@ -8437,7 +9505,7 @@
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="33"/>
-      <c r="G13" s="68"/>
+      <c r="G13" s="75"/>
       <c r="J13">
         <f>8.07/0.09</f>
         <v>89.666666666666671</v>
@@ -8463,7 +9531,7 @@
       </c>
       <c r="E14" s="33"/>
       <c r="F14" s="33"/>
-      <c r="G14" s="68"/>
+      <c r="G14" s="75"/>
       <c r="J14">
         <f>1060/J13</f>
         <v>11.821561338289962</v>
@@ -8531,19 +9599,19 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A41" s="62" t="s">
+      <c r="A41" s="54" t="s">
         <v>314</v>
       </c>
-      <c r="B41" s="62"/>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="62"/>
-      <c r="G41" s="62"/>
-      <c r="H41" s="62"/>
-      <c r="I41" s="62"/>
-      <c r="J41" s="62"/>
-      <c r="K41" s="62"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="54"/>
+      <c r="K41" s="54"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -8578,7 +9646,7 @@
         <f>1/8.07</f>
         <v>0.12391573729863692</v>
       </c>
-      <c r="G47" s="61" t="s">
+      <c r="G47" s="58" t="s">
         <v>289</v>
       </c>
     </row>
@@ -8597,7 +9665,7 @@
         <f>1.06*E47</f>
         <v>0.13135068153655513</v>
       </c>
-      <c r="G48" s="61"/>
+      <c r="G48" s="58"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -8614,7 +9682,7 @@
         <f>E48*1.1</f>
         <v>0.14448574969021066</v>
       </c>
-      <c r="G49" s="61"/>
+      <c r="G49" s="58"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -8630,7 +9698,7 @@
       <c r="E50">
         <v>6</v>
       </c>
-      <c r="G50" s="61"/>
+      <c r="G50" s="58"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -8661,16 +9729,16 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D54" s="39"/>
-      <c r="E54" s="69" t="s">
+      <c r="E54" s="76" t="s">
         <v>290</v>
       </c>
-      <c r="F54" s="69"/>
-      <c r="G54" s="69"/>
-      <c r="H54" s="70" t="s">
+      <c r="F54" s="76"/>
+      <c r="G54" s="76"/>
+      <c r="H54" s="77" t="s">
         <v>294</v>
       </c>
-      <c r="I54" s="70"/>
-      <c r="J54" s="70"/>
+      <c r="I54" s="77"/>
+      <c r="J54" s="77"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -8853,29 +9921,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="80" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="K1" s="71" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="K1" s="78" t="s">
         <v>222</v>
       </c>
       <c r="L1" t="s">
         <v>156</v>
       </c>
-      <c r="S1" s="71" t="s">
+      <c r="S1" s="78" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="K2" s="71"/>
+      <c r="K2" s="78"/>
       <c r="M2" t="s">
         <v>225</v>
       </c>
@@ -8885,21 +9953,21 @@
       <c r="O2" t="s">
         <v>227</v>
       </c>
-      <c r="S2" s="71"/>
+      <c r="S2" s="78"/>
     </row>
     <row r="3" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="79" t="s">
         <v>220</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="K3" s="78"/>
       <c r="L3" t="s">
         <v>159</v>
       </c>
@@ -8912,7 +9980,7 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="S3" s="71"/>
+      <c r="S3" s="78"/>
       <c r="T3" t="s">
         <v>159</v>
       </c>
@@ -8937,7 +10005,7 @@
       <c r="E4" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="K4" s="71"/>
+      <c r="K4" s="78"/>
       <c r="L4" t="s">
         <v>158</v>
       </c>
@@ -8952,7 +10020,7 @@
         <f>N4/SUM(N$4:N$6)</f>
         <v>0.5</v>
       </c>
-      <c r="S4" s="71"/>
+      <c r="S4" s="78"/>
       <c r="T4" t="s">
         <v>158</v>
       </c>
@@ -8979,7 +10047,7 @@
       <c r="I5" t="s">
         <v>237</v>
       </c>
-      <c r="K5" s="71"/>
+      <c r="K5" s="78"/>
       <c r="L5" t="s">
         <v>160</v>
       </c>
@@ -8994,7 +10062,7 @@
         <f>N5/SUM(N$4:N$6)</f>
         <v>0.47058823529411764</v>
       </c>
-      <c r="S5" s="71"/>
+      <c r="S5" s="78"/>
       <c r="T5" t="s">
         <v>160</v>
       </c>
@@ -9025,7 +10093,7 @@
         <f>E6*D6</f>
         <v>1.0043063938618926</v>
       </c>
-      <c r="K6" s="71"/>
+      <c r="K6" s="78"/>
       <c r="L6" t="s">
         <v>161</v>
       </c>
@@ -9040,7 +10108,7 @@
         <f t="shared" si="1"/>
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="S6" s="71"/>
+      <c r="S6" s="78"/>
       <c r="T6" t="s">
         <v>161</v>
       </c>
@@ -9176,17 +10244,17 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="79" t="s">
         <v>232</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
       <c r="T13" t="s">
         <v>161</v>
       </c>
@@ -9332,17 +10400,17 @@
       </c>
     </row>
     <row r="23" spans="1:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="72" t="s">
+      <c r="A23" s="79" t="s">
         <v>231</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
       <c r="O23" s="23" t="s">
         <v>239</v>
       </c>
@@ -9678,17 +10746,17 @@
       </c>
     </row>
     <row r="33" spans="1:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="A33" s="72" t="s">
+      <c r="A33" s="79" t="s">
         <v>229</v>
       </c>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="79"/>
+      <c r="I33" s="79"/>
       <c r="O33" s="23" t="s">
         <v>239</v>
       </c>
@@ -10188,17 +11256,17 @@
       </c>
     </row>
     <row r="54" spans="1:24" ht="31" x14ac:dyDescent="0.2">
-      <c r="A54" s="73" t="s">
+      <c r="A54" s="80" t="s">
         <v>281</v>
       </c>
-      <c r="B54" s="73"/>
-      <c r="C54" s="73"/>
-      <c r="D54" s="73"/>
-      <c r="E54" s="73"/>
-      <c r="F54" s="73"/>
-      <c r="G54" s="73"/>
-      <c r="H54" s="73"/>
-      <c r="I54" s="73"/>
+      <c r="B54" s="80"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="80"/>
+      <c r="G54" s="80"/>
+      <c r="H54" s="80"/>
+      <c r="I54" s="80"/>
       <c r="O54" s="23" t="s">
         <v>239</v>
       </c>
@@ -10235,17 +11303,17 @@
       </c>
     </row>
     <row r="56" spans="1:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="A56" s="72" t="s">
+      <c r="A56" s="79" t="s">
         <v>282</v>
       </c>
-      <c r="B56" s="72"/>
-      <c r="C56" s="72"/>
-      <c r="D56" s="72"/>
-      <c r="E56" s="72"/>
-      <c r="F56" s="72"/>
-      <c r="G56" s="72"/>
-      <c r="H56" s="72"/>
-      <c r="I56" s="72"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="79"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="79"/>
+      <c r="F56" s="79"/>
+      <c r="G56" s="79"/>
+      <c r="H56" s="79"/>
+      <c r="I56" s="79"/>
       <c r="O56" s="23" t="s">
         <v>239</v>
       </c>
@@ -10376,7 +11444,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="59" t="s">
         <v>190</v>
       </c>
       <c r="B1" t="s">
@@ -10385,28 +11453,28 @@
       <c r="C1" s="34">
         <v>36.4</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="81" t="s">
         <v>194</v>
       </c>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="N1" s="75" t="s">
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="N1" s="82" t="s">
         <v>193</v>
       </c>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
       <c r="U1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="53"/>
+      <c r="A2" s="59"/>
       <c r="B2" t="s">
         <v>189</v>
       </c>
@@ -10427,7 +11495,7 @@
       <c r="S2" s="36"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="53"/>
+      <c r="A3" s="59"/>
       <c r="B3" t="s">
         <v>162</v>
       </c>
@@ -10882,14 +11950,14 @@
       <c r="S29" s="36"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G30" s="61" t="s">
+      <c r="G30" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="H30" s="61"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="61"/>
-      <c r="K30" s="61"/>
-      <c r="L30" s="61"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
       <c r="N30" s="36"/>
       <c r="O30" s="36"/>
       <c r="P30" s="36"/>
@@ -10922,14 +11990,14 @@
       <c r="S33" s="36"/>
     </row>
     <row r="34" spans="14:19" x14ac:dyDescent="0.2">
-      <c r="N34" s="61" t="s">
+      <c r="N34" s="58" t="s">
         <v>191</v>
       </c>
-      <c r="O34" s="61"/>
-      <c r="P34" s="61"/>
-      <c r="Q34" s="61"/>
-      <c r="R34" s="61"/>
-      <c r="S34" s="61"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="58"/>
+      <c r="R34" s="58"/>
+      <c r="S34" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>